<commit_message>
New risks and AI Stages
</commit_message>
<xml_diff>
--- a/data/risk_matrix.xlsx
+++ b/data/risk_matrix.xlsx
@@ -5,13 +5,16 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Please check again all sources " sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - risk_matrix v2" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="211">
+  <si>
+    <t>risk_matrix v2</t>
+  </si>
   <si>
     <t>Process Name</t>
   </si>
@@ -28,6 +31,9 @@
     <t>Sources and References</t>
   </si>
   <si>
+    <t>NIST AI Lifecycle Stage</t>
+  </si>
+  <si>
     <t>1. AI Strategy &amp; Value Mgmt.</t>
   </si>
   <si>
@@ -40,7 +46,10 @@
     <t>Pursuing disruptive AI ambitions without the requisite technology maturity, data readiness, or organizational buy-in, leading to project failure.</t>
   </si>
   <si>
-    <t>Gartner: AI Roadmap; Gartner: AI Strategy; ISO/IEC 42001 (Context of Org)</t>
+    <t>Gartner: AI Roadmap; Gartner: AI Strategy; ISO/IEC 42001 (Context of Org); NIST AI RMF: MAP 1.1, MAP 1.2</t>
+  </si>
+  <si>
+    <t>Plan &amp; Design</t>
   </si>
   <si>
     <t>Competitive Race Risk</t>
@@ -49,7 +58,7 @@
     <t>Rapidly deploying AI systems to maximize strategic advantage, prioritizing speed over safety or diligence (The "AI Race").</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 6.4 (Competitive Dynamics); Gartner: Risk Essentials</t>
+    <t>MIT AI Risk Rep: 6.4 (Competitive Dynamics); Gartner: Risk Essentials; NIST AI RMF: GOVERN 1.2, MAP 1.5</t>
   </si>
   <si>
     <t>Strategic Misalignment</t>
@@ -58,7 +67,7 @@
     <t>AI initiatives do not deliver on key strategic goals, fail to adapt to business priorities, or are disconnected from the broader business strategy.</t>
   </si>
   <si>
-    <t>Gartner: AI Strategy; MITRE: Strategy &amp; Resources; ISO/IEC 42001 (Leadership)</t>
+    <t>Gartner: AI Strategy; MITRE: Strategy &amp; Resources; ISO/IEC 42001 (Leadership); NIST AI RMF: GOVERN 1.1, GOVERN 1.3</t>
   </si>
   <si>
     <t>Proxy Gaming (Reward Hacking)</t>
@@ -67,7 +76,7 @@
     <t>The AI system optimizes for a proxy metric (e.g., clicks, engagement) at the expense of the true strategic goal, leading to distorted outcomes.</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 7.1 (Goal Misalignment); Gartner: AI Value</t>
+    <t>MIT AI Risk Rep: 7.1 (Goal Misalignment); Gartner: AI Value; NIST AI RMF: MAP 1.1, MEASURE 2.1</t>
   </si>
   <si>
     <t>Portfolio Management</t>
@@ -79,7 +88,7 @@
     <t>The process for selecting AI projects does not align with strategic goals, value potential, or feasibility (e.g., failing to distinguish between "Defend," "Extend," and "Upend").</t>
   </si>
   <si>
-    <t>Gartner: AI Value; Gartner: AI Roadmap; MITRE: Strategy</t>
+    <t>Gartner: AI Value; Gartner: AI Roadmap; MITRE: Strategy; NIST AI RMF: MAP 1.3, MAP 1.4</t>
   </si>
   <si>
     <t>Value Realization</t>
@@ -91,7 +100,7 @@
     <t>Inability to measure tangible benefits due to a lack of clear metrics, productivity leaks, or failure to reinvest time saved.</t>
   </si>
   <si>
-    <t>Gartner: AI Value (Metrics); Gartner: AI Roadmap; Gartner: AI People &amp; Culture</t>
+    <t>Gartner: AI Value (Metrics); Gartner: AI Roadmap; Gartner: AI People &amp; Culture; NIST AI RMF: MEASURE 1.1, MANAGE 4.2</t>
   </si>
   <si>
     <t>Financial Management</t>
@@ -103,7 +112,16 @@
     <t>Excessive costs from AI services (API calls, compute) or malicious Model Denial of Service attacks causing resource exhaustion.</t>
   </si>
   <si>
-    <t>Gartner: AI Value (FinOps); OWASP LLM Top 10: LLM04; ISO/IEC 42001</t>
+    <t>Gartner: AI Value (FinOps); OWASP LLM Top 10: LLM04; ISO/IEC 42001; NIST AI RMF: GOVERN 1.3, MANAGE 4.3</t>
+  </si>
+  <si>
+    <t>Pseudoscience / Scientific Invalidity</t>
+  </si>
+  <si>
+    <t>The AI is tasked with predicting something that cannot scientifically be predicted (e.g., physiognomy, predicting criminality from facial features), leading to fundamentally invalid results.</t>
+  </si>
+  <si>
+    <t>NIST AI RMF: MEASURE 2.2 (Validity), MAP 1.2 (Scientific Integrity); Princeton AI Snake Oil</t>
   </si>
   <si>
     <t>2. AI Organization &amp; Culture</t>
@@ -118,7 +136,7 @@
     <t>The rapid evolution of AI capabilities outpaces the organization's ability to adopt them due to siloed structures or lack of cross-functional collaboration.</t>
   </si>
   <si>
-    <t>Gartner: AI Roadmap; Gartner: AI Strategy; MITRE: Organization</t>
+    <t>Gartner: AI Roadmap; Gartner: AI Strategy; MITRE: Organization; NIST AI RMF: GOVERN 1.2, GOVERN 2.2</t>
   </si>
   <si>
     <t>Roles &amp; Responsibilities</t>
@@ -130,7 +148,7 @@
     <t>Roles for AI development, oversight, and "human-in-the-loop" decision rights are not clearly defined, leading to responsibility gaps.</t>
   </si>
   <si>
-    <t>Gartner: AI Organization; MITRE: Org Structure; ISO/IEC 42001 (Roles A.3.2)</t>
+    <t>Gartner: AI Organization; MITRE: Org Structure; ISO/IEC 42001 (Roles A.3.2); NIST AI RMF: GOVERN 2.1, GOVERN 2.3</t>
   </si>
   <si>
     <t>Talent Management</t>
@@ -142,7 +160,7 @@
     <t>The inability to hire, develop, or retain talent with necessary niche technical skills (e.g., data scientists, prompt engineers) hinders strategy execution.</t>
   </si>
   <si>
-    <t>Gartner: AI Organization; Gartner: AI Engineering (Skills)</t>
+    <t>Gartner: AI Organization; Gartner: AI Engineering (Skills); NIST AI RMF: GOVERN 2.2</t>
   </si>
   <si>
     <t>Workforce Transformation</t>
@@ -154,7 +172,7 @@
     <t>Insufficient AI literacy across the general workforce prevents effective adoption, leads to poor decision-making, or results in accidental misuse.</t>
   </si>
   <si>
-    <t>Gartner: AI Literacy Roadmap; ISO/IEC 42001 (Competence 7.2); MITRE: Workforce</t>
+    <t>Gartner: AI Literacy Roadmap; ISO/IEC 42001 (Competence 7.2); MITRE: Workforce; NIST AI RMF: GOVERN 2.2</t>
   </si>
   <si>
     <t>Overreliance &amp; Loss of Agency</t>
@@ -163,7 +181,10 @@
     <t>Users accepting AI results without verification or delegating too much control, leading to loss of human agency or Anthropomorphism.</t>
   </si>
   <si>
-    <t>OWASP LLM Top 10: LLM09; MIT AI Risk Rep: 5.2; Gartner: AI People &amp; Culture</t>
+    <t>OWASP LLM Top 10: LLM09; MIT AI Risk Rep: 5.2; Gartner: AI People &amp; Culture; NIST AI RMF: MAP 1.1, MANAGE 3.2</t>
+  </si>
+  <si>
+    <t>Use</t>
   </si>
   <si>
     <t>User Resistance &amp; Adoption Failure</t>
@@ -172,7 +193,7 @@
     <t>End-users fail to adopt AI tools due to poor user experience (UX), lack of trust, misalignment with workflows, or passive resistance.</t>
   </si>
   <si>
-    <t>MITRE: Usage &amp; Adoption; Gartner: AI People &amp; Culture; ISO/IEC 42001 (Awareness)</t>
+    <t>MITRE: Usage &amp; Adoption; Gartner: AI People &amp; Culture; ISO/IEC 42001 (Awareness); NIST AI RMF: GOVERN 5.2</t>
   </si>
   <si>
     <t>Workforce Disruption</t>
@@ -181,7 +202,7 @@
     <t>Fear of job replacement or significant role changes leads to low morale, distrust, active resistance, or cultural devaluation of human effort.</t>
   </si>
   <si>
-    <t>Gartner: AI People &amp; Culture; MITRE: Culture; MIT AI Risk Rep: 6.2</t>
+    <t>Gartner: AI People &amp; Culture; MITRE: Culture; MIT AI Risk Rep: 6.2; NIST AI RMF: GOVERN 1.2, MAP 1.1</t>
   </si>
   <si>
     <t>Cultural Devaluation of Human Effort</t>
@@ -190,7 +211,7 @@
     <t>The devaluation of human creativity, skills, and innovation (e.g., art, writing) due to the ubiquity of AI-generated content.</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 6.3 (Cultural Devaluation); Gartner: AI People &amp; Culture</t>
+    <t>MIT AI Risk Rep: 6.3 (Cultural Devaluation); Gartner: AI People &amp; Culture; NIST AI RMF: MAP 1.1</t>
   </si>
   <si>
     <t>3. AI Governance &amp; Risk</t>
@@ -205,7 +226,7 @@
     <t>The organization lacks a formalized AI risk and compliance framework (or the existing one is insufficient) to manage obligations.</t>
   </si>
   <si>
-    <t>Gartner: AI Governance; MITRE: Governance; ISO/IEC 42001 (Clause 4.4, A.2)</t>
+    <t>Gartner: AI Governance; MITRE: Governance; ISO/IEC 42001 (Clause 4.4, A.2); NIST AI RMF: GOVERN 1.1, GOVERN 2.1</t>
   </si>
   <si>
     <t>Missing AI Inventory (Shadow AI)</t>
@@ -214,7 +235,7 @@
     <t>Failure to maintain a comprehensive inventory of all AI systems, use cases, and models prevents effective oversight and compliance.</t>
   </si>
   <si>
-    <t>Gartner: AI Governance (Inventory); ISO/IEC 5338; ISO/IEC 42001 (Resources A.4.2)</t>
+    <t>Gartner: AI Governance (Inventory); ISO/IEC 5338; ISO/IEC 42001 (Resources A.4.2); NIST AI RMF: MAP 2.1, MANAGE 1.1</t>
   </si>
   <si>
     <t>Ineffective AI System Classification</t>
@@ -223,7 +244,7 @@
     <t>Failure to accurately classify AI systems by risk level (e.g., High, Limited, Minimal) leads to inappropriate controls or regulatory non-compliance.</t>
   </si>
   <si>
-    <t>ISO/IEC 42001 (Impact Assessment A.5.2); Gartner: AI Governance; MITRE: Ethical Use</t>
+    <t>ISO/IEC 42001 (Impact Assessment A.5.2); Gartner: AI Governance; MITRE: Ethical Use; NIST AI RMF: MAP 1.5, MAP 2.2</t>
   </si>
   <si>
     <t>Shadow AI (Unmanaged Procurement)</t>
@@ -232,7 +253,7 @@
     <t>Business units purchasing or using AI tools without authorized oversight, leading to "SaaS sprawl" and unmanaged data risks.</t>
   </si>
   <si>
-    <t>Gartner: AI Roadmap; Gartner: AI Governance; ISO/IEC 42001; Gartner: Risk Essentials</t>
+    <t>Gartner: AI Roadmap; Gartner: AI Governance; ISO/IEC 42001; Gartner: Risk Essentials; NIST AI RMF: GOVERN 1.1, MANAGE 1.3</t>
   </si>
   <si>
     <t>Legal &amp; Compliance</t>
@@ -244,7 +265,7 @@
     <t>Failure to comply with emerging regulations (e.g., EU AI Act, US Executive Orders) creates significant legal, financial, and reputational exposure.</t>
   </si>
   <si>
-    <t>Gartner: AI Governance (Legal); Gartner: AI Strategy; ISO/IEC 42001 (Context)</t>
+    <t>Gartner: AI Governance (Legal); Gartner: AI Strategy; ISO/IEC 42001 (Context); NIST AI RMF: GOVERN 1.1, MAP 1.1</t>
   </si>
   <si>
     <t>AI Supply Chain &amp; Third-Party Risk</t>
@@ -253,7 +274,10 @@
     <t>Vulnerabilities in the AI supply chain, including compromised third-party models, training data, or ambiguity in vendor contracts.</t>
   </si>
   <si>
-    <t>OWASP LLM Top 10: LLM05; OWASP ML Top 10: ML06; ISO/IEC 42001 (Suppliers A.10.3)</t>
+    <t>OWASP LLM Top 10: LLM05; OWASP ML Top 10: ML06; ISO/IEC 42001 (Suppliers A.10.3); NIST AI RMF: MANAGE 1.3, MAP 2.3</t>
+  </si>
+  <si>
+    <t>Collect &amp; Process Data</t>
   </si>
   <si>
     <t>Intellectual Property Infringement</t>
@@ -262,7 +286,7 @@
     <t>Training data or model outputs violate copyright laws, leading to litigation or loss of ownership over generated assets.</t>
   </si>
   <si>
-    <t>Gartner: AI Governance (Legal); MIT AI Risk Rep: 6.3</t>
+    <t>Gartner: AI Governance (Legal); MIT AI Risk Rep: 6.3; NIST AI RMF: GOVERN 1.1, MAP 1.1</t>
   </si>
   <si>
     <t>4. AI Data Management</t>
@@ -277,7 +301,7 @@
     <t>Using data that is technically accurate but essentially "wrong" for the specific AI use case or context, leading to misleading outputs.</t>
   </si>
   <si>
-    <t>Gartner: AI Data Guide; ISO/IEC 5338; MITRE: Data</t>
+    <t>Gartner: AI Data Guide; ISO/IEC 5338; MITRE: Data; NIST AI RMF: MAP 2.3, MEASURE 2.2</t>
   </si>
   <si>
     <t>Metadata Management Failure</t>
@@ -286,7 +310,7 @@
     <t>Treating metadata as documentation rather than infrastructure, leading to an inability to explain model behavior or track lineage (Provenance).</t>
   </si>
   <si>
-    <t>Gartner: AI Data Guide; ISO/IEC 5338; ISO/IEC 42001 (Provenance A.7.5)</t>
+    <t>Gartner: AI Data Guide; ISO/IEC 5338; ISO/IEC 42001 (Provenance A.7.5); NIST AI RMF: MAP 2.3</t>
   </si>
   <si>
     <t>Static Data Mindset (Model Collapse)</t>
@@ -295,7 +319,7 @@
     <t>Treating data readiness as a one-time checklist, potentially leading to model collapse if trained on synthetic data loops or drift.</t>
   </si>
   <si>
-    <t>Gartner: AI Data Guide; Gartner: Risk Essentials; MIT AI Risk Rep</t>
+    <t>Gartner: AI Data Guide; Gartner: Risk Essentials; MIT AI Risk Rep; NIST AI RMF: MANAGE 4.1, MANAGE 4.2</t>
   </si>
   <si>
     <t>Privacy &amp; Security</t>
@@ -307,7 +331,7 @@
     <t>Exposure of PII/IP via Model Inversion, Membership Inference, or memorization of sensitive training data.</t>
   </si>
   <si>
-    <t>OWASP LLM Top 10: LLM06; OWASP ML Top 10: ML03, ML04; ISO/IEC 42001 (Privacy B.7.2)</t>
+    <t>OWASP LLM Top 10: LLM06; OWASP ML Top 10: ML03, ML04; ISO/IEC 42001 (Privacy B.7.2); NIST AI RMF: MEASURE 2.7, MANAGE 2.4</t>
   </si>
   <si>
     <t>5. AI Engineering &amp; Lifecycle</t>
@@ -322,7 +346,10 @@
     <t>Inability to move from successful pilots to enterprise-scale production due to technical incompatibility or architectural complexity.</t>
   </si>
   <si>
-    <t>Gartner: AI Roadmap; Gartner: AI Engineering</t>
+    <t>Gartner: AI Roadmap; Gartner: AI Engineering; NIST AI RMF: MANAGE 2.2</t>
+  </si>
+  <si>
+    <t>Build</t>
   </si>
   <si>
     <t>Inadequate Verification &amp; Validation</t>
@@ -331,7 +358,10 @@
     <t>Failure to rigorously test AI models for accuracy, robustness, bias, and security prior to deployment, leading to performance failures.</t>
   </si>
   <si>
-    <t>ISO/IEC 5338 (Verification); ISO/IEC 42001 (Control A.6.2.4); MITRE: Test &amp; Evaluation</t>
+    <t>ISO/IEC 5338 (Verification); ISO/IEC 42001 (Control A.6.2.4); MITRE: Test &amp; Evaluation; NIST AI RMF: MEASURE 1.1, MEASURE 2.6</t>
+  </si>
+  <si>
+    <t>Verify &amp; Validate</t>
   </si>
   <si>
     <t>Insecure Output Handling</t>
@@ -340,7 +370,7 @@
     <t>Downstream components blindly accepting AI output without validation, leading to XSS, CSRF, or code execution vulnerabilities.</t>
   </si>
   <si>
-    <t>OWASP LLM Top 10: LLM02; OWASP ML Top 10: ML09</t>
+    <t>OWASP LLM Top 10: LLM02; OWASP ML Top 10: ML09; NIST AI RMF: MANAGE 2.5, MEASURE 2.6</t>
   </si>
   <si>
     <t>Insecure Plugin &amp; Tool Design</t>
@@ -349,7 +379,7 @@
     <t>AI plugins or tools accepting unsafe inputs or possessing insecure access controls, enabling malicious actions.</t>
   </si>
   <si>
-    <t>OWASP LLM Top 10: LLM07; Gartner: AI Engineering; ISO/IEC 42001 (Tooling A.4.4)</t>
+    <t>OWASP LLM Top 10: LLM07; Gartner: AI Engineering; ISO/IEC 42001 (Tooling A.4.4); NIST AI RMF: MANAGE 1.3, MANAGE 2.5</t>
   </si>
   <si>
     <t>Operations &amp; Maintenance</t>
@@ -361,7 +391,10 @@
     <t>The degradation of model performance over time as real-world data diverges from training data (Data/Concept Drift).</t>
   </si>
   <si>
-    <t>Gartner: AI Engineering; MITRE: Solution Monitoring; OWASP ML Top 10: ML08</t>
+    <t>Gartner: AI Engineering; MITRE: Solution Monitoring; OWASP ML Top 10: ML08; NIST AI RMF: MANAGE 4.2, MEASURE 2.12</t>
+  </si>
+  <si>
+    <t>Operate &amp; Monitor</t>
   </si>
   <si>
     <t>Continuous Validation Failure</t>
@@ -370,7 +403,7 @@
     <t>Failure to implement continuous monitoring to detect drift, security vulnerabilities, or performance degradation in deployed models.</t>
   </si>
   <si>
-    <t>ISO/IEC 5338; ISO/IEC 42001 (Monitoring A.6.2.6); MITRE: Solution Monitoring</t>
+    <t>ISO/IEC 5338; ISO/IEC 42001 (Monitoring A.6.2.6); MITRE: Solution Monitoring; NIST AI RMF: MANAGE 4.1, MANAGE 4.2</t>
   </si>
   <si>
     <t>Ineffective AI Change Management</t>
@@ -379,7 +412,7 @@
     <t>Change management processes fail to account for AI specificities (e.g., prompt versioning, model retraining, weight updates), leading to regression.</t>
   </si>
   <si>
-    <t>ISO/IEC 42001 (Clause 6.3); ISO/IEC 5338; Gartner: AI Engineering (ModelOps)</t>
+    <t>ISO/IEC 42001 (Clause 6.3); ISO/IEC 5338; Gartner: AI Engineering (ModelOps); NIST AI RMF: MANAGE 3.1</t>
   </si>
   <si>
     <t>Inadequate AI Incident Response</t>
@@ -388,7 +421,7 @@
     <t>Lack of specific protocols to detect, contain, and recover from AI-specific incidents (e.g., adversarial attacks, unintended outputs).</t>
   </si>
   <si>
-    <t>ISO/IEC 42001 (Clause A.8.4); Gartner: Risk Essentials; OWASP LLM Top 10</t>
+    <t>ISO/IEC 42001 (Clause A.8.4); Gartner: Risk Essentials; OWASP LLM Top 10; NIST AI RMF: MANAGE 4.3</t>
   </si>
   <si>
     <t>Insufficient AI Logging &amp; Forensics</t>
@@ -397,7 +430,7 @@
     <t>Lack of comprehensive event logging prevents forensic investigation of AI incidents, model failures, or adversarial attacks.</t>
   </si>
   <si>
-    <t>ISO/IEC 42001 (Event Logs A.6.2.8); OWASP LLM Top 10</t>
+    <t>ISO/IEC 42001 (Event Logs A.6.2.8); OWASP LLM Top 10; NIST AI RMF: MANAGE 4.2, MEASURE 2.1</t>
   </si>
   <si>
     <t>Improper Decommissioning</t>
@@ -406,7 +439,16 @@
     <t>Risks associated with the retirement of AI systems, including residual sensitive data retention or security gaps during sunsetting.</t>
   </si>
   <si>
-    <t>ISO/IEC 5338 (Lifecycle Processes); ISO/IEC 42001 (Resources A.4.6)</t>
+    <t>ISO/IEC 5338 (Lifecycle Processes); ISO/IEC 42001 (Resources A.4.6); NIST AI RMF: MANAGE 3.3</t>
+  </si>
+  <si>
+    <t>Off-Label / Unintended Use</t>
+  </si>
+  <si>
+    <t>Legitimate users utilizing the system for a purpose it was not designed, tested, or validated for (e.g., medical advice from a general coding bot), leading to harm.</t>
+  </si>
+  <si>
+    <t>NIST AI RMF: MAP 1.2, MAP 1.5 (Risk Tolerance), MANAGE 4.1</t>
   </si>
   <si>
     <t>6. AI Security &amp; Malicious Use</t>
@@ -421,7 +463,7 @@
     <t>Crafting adversarial inputs to manipulate model behavior, bypass filters, or execute unauthorized actions.</t>
   </si>
   <si>
-    <t>OWASP LLM Top 10: LLM01; OWASP ML Top 10: ML01; Gartner: AI Governance</t>
+    <t>OWASP LLM Top 10: LLM01; OWASP ML Top 10: ML01; Gartner: AI Governance; NIST AI RMF: MANAGE 2.5, MEASURE 2.6</t>
   </si>
   <si>
     <t>Data &amp; Training Poisoning</t>
@@ -430,7 +472,7 @@
     <t>Manipulating training data or fine-tuning processes to introduce backdoors, biases, or vulnerabilities (e.g., Neural Trojans).</t>
   </si>
   <si>
-    <t>OWASP LLM Top 10: LLM03; OWASP ML Top 10: ML02, ML10; Gartner: Risk Essentials</t>
+    <t>OWASP LLM Top 10: LLM03; OWASP ML Top 10: ML02, ML10; Gartner: Risk Essentials; NIST AI RMF: MANAGE 2.5, MEASURE 2.6</t>
   </si>
   <si>
     <t>Model Theft &amp; IP Extraction</t>
@@ -439,7 +481,7 @@
     <t>Unauthorized exfiltration of model weights, architecture, or proprietary parameters to replicate or reverse-engineer the system.</t>
   </si>
   <si>
-    <t>OWASP LLM Top 10: LLM10; OWASP ML Top 10: ML05, ML07; ISO/IEC 42001 (Security B.9.2)</t>
+    <t>OWASP LLM Top 10: LLM10; OWASP ML Top 10: ML05, ML07; ISO/IEC 42001 (Security B.9.2); NIST AI RMF: MANAGE 2.5, MEASURE 2.6</t>
   </si>
   <si>
     <t>Malicious Application</t>
@@ -451,7 +493,7 @@
     <t>Actors using AI for large-scale disinformation, surveillance, fraud, deepfakes, or targeted manipulation of beliefs.</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 4.1, 4.2; Gartner: Risk Essentials</t>
+    <t>MIT AI Risk Rep: 4.1, 4.2; Gartner: Risk Essentials; NIST AI RMF: MAP 1.1, MEASURE 2.5</t>
   </si>
   <si>
     <t>AI-Enabled Cyber Warfare</t>
@@ -460,7 +502,7 @@
     <t>Using AI systems to develop cyber weapons (e.g., coding cheaper malware) or enhance existing weapons to cause mass harm.</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 4.3; Gartner: Risk Essentials</t>
+    <t>MIT AI Risk Rep: 4.3; Gartner: Risk Essentials; NIST AI RMF: MAP 1.1</t>
   </si>
   <si>
     <t>7. Societal &amp; Ethical Impact</t>
@@ -475,7 +517,7 @@
     <t>The model produces factually incorrect results that users accept as truth, compromising decision-making and eroding trust.</t>
   </si>
   <si>
-    <t>Gartner: AI Governance; MITRE: Robust &amp; Reliable; MIT AI Risk Rep: 3.1</t>
+    <t>Gartner: AI Governance; MITRE: Robust &amp; Reliable; MIT AI Risk Rep: 3.1; NIST AI RMF: MEASURE 2.3</t>
   </si>
   <si>
     <t>Sycophancy</t>
@@ -484,7 +526,7 @@
     <t>The AI generates responses that align with the user's existing beliefs or biases rather than providing objective facts.</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 3.1; Gartner: AI Governance</t>
+    <t>MIT AI Risk Rep: 3.1; Gartner: AI Governance; NIST AI RMF: MEASURE 2.2</t>
   </si>
   <si>
     <t>Lack of Explainability (Black Box)</t>
@@ -493,7 +535,7 @@
     <t>The AI system functions as a "black box," making it impossible to understand, justify, or contest its decisions, leading to loss of trust.</t>
   </si>
   <si>
-    <t>NIST AI RMF; Gartner: AI Governance; MIT AI Risk Rep: 5.1; ISO/IEC 42001 (Transparency)</t>
+    <t>NIST AI RMF; Gartner: AI Governance; MIT AI Risk Rep: 5.1; ISO/IEC 42001 (Transparency); NIST AI RMF: MEASURE 2.9, GOVERN 5.2</t>
   </si>
   <si>
     <t>Inadequate System Documentation</t>
@@ -502,7 +544,7 @@
     <t>Users lack sufficient instructions (technical/usage) to operate the AI system safely or understand its limitations, leading to misuse.</t>
   </si>
   <si>
-    <t>ISO/IEC 42001 (Documentation A.8.2); Gartner: AI Governance</t>
+    <t>ISO/IEC 42001 (Documentation A.8.2); Gartner: AI Governance; NIST AI RMF: GOVERN 4.2, MAP 2.2</t>
   </si>
   <si>
     <t>Pollution of Information Ecosystem</t>
@@ -511,7 +553,7 @@
     <t>AI generating personalized misinformation or "slop," creating filter bubbles and undermining shared reality or consensus.</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 3.2; Gartner: Risk Essentials</t>
+    <t>MIT AI Risk Rep: 3.2; Gartner: Risk Essentials; NIST AI RMF: MAP 1.1</t>
   </si>
   <si>
     <t>Toxic Content Exposure</t>
@@ -520,7 +562,16 @@
     <t>AI exposing users to harmful, abusive, unsafe, or inappropriate content (e.g., hate speech, violence, extremism).</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 1.2; Gartner: AI Governance</t>
+    <t>MIT AI Risk Rep: 1.2; Gartner: AI Governance; NIST AI RMF: MEASURE 2.5, MANAGE 2.3</t>
+  </si>
+  <si>
+    <t>Lack of Recourse &amp; Redress</t>
+  </si>
+  <si>
+    <t>Individuals impacted by an adverse AI decision (e.g., loan denial, fraud flag) have no mechanism to appeal, challenge, or correct the decision.</t>
+  </si>
+  <si>
+    <t>NIST AI RMF: GOVERN 1.6, MANAGE 4.1; EU AI Act (Article 86)</t>
   </si>
   <si>
     <t>Fairness &amp; Bias</t>
@@ -532,7 +583,7 @@
     <t>The model's outputs reflect societal or data-driven biases, systematically disadvantaging certain demographic groups.</t>
   </si>
   <si>
-    <t>Gartner: AI Governance (Ethics); MITRE: Human-Centric; ISO/IEC 42001 (Fairness A.5.4); MIT AI Risk Rep: 1.1</t>
+    <t>Gartner: AI Governance (Ethics); MITRE: Human-Centric; ISO/IEC 42001 (Fairness A.5.4); MIT AI Risk Rep: 1.1; NIST AI RMF: MEASURE 2.2, MANAGE 2.3</t>
   </si>
   <si>
     <t>Socioeconomic Inequality</t>
@@ -541,7 +592,7 @@
     <t>AI-driven concentration of power, unfair distribution of benefits, or exacerbation of existing inequalities.</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 6.1; Gartner: AI Governance; ISO/IEC 42001 (Societal Impact A.5.5)</t>
+    <t>MIT AI Risk Rep: 6.1; Gartner: AI Governance; ISO/IEC 42001 (Societal Impact A.5.5); NIST AI RMF: MAP 1.1, GOVERN 1.2</t>
   </si>
   <si>
     <t>Safety &amp; Alignment</t>
@@ -553,7 +604,7 @@
     <t>Autonomous agents taking unintended actions (Excessive Agency) due to ambiguous permissions or lack of human oversight.</t>
   </si>
   <si>
-    <t>OWASP LLM Top 10: LLM08; Gartner: AI Governance (Agentic); MIT AI Risk Rep: 7.6</t>
+    <t>OWASP LLM Top 10: LLM08; Gartner: AI Governance (Agentic); MIT AI Risk Rep: 7.6; NIST AI RMF: MAP 1.1, MANAGE 3.2</t>
   </si>
   <si>
     <t>Goal Misalignment</t>
@@ -562,7 +613,7 @@
     <t>AI systems acting in conflict with human goals/values, potentially using capabilities like deception or seeking power/resources.</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 7.1; Gartner: AI Ethics</t>
+    <t>MIT AI Risk Rep: 7.1; Gartner: AI Ethics; NIST AI RMF: MAP 1.1, MEASURE 2.1</t>
   </si>
   <si>
     <t>Emergent Dangerous Capabilities</t>
@@ -571,7 +622,7 @@
     <t>Unanticipated capabilities arising in large models (e.g., self-proliferation, sophisticated deception) that pose safety risks.</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 7.2; Gartner: AI Strategy</t>
+    <t>MIT AI Risk Rep: 7.2; Gartner: AI Strategy; NIST AI RMF: MEASURE 2.6, MANAGE 4.1</t>
   </si>
   <si>
     <t>AI Welfare &amp; Rights</t>
@@ -580,7 +631,7 @@
     <t>Ethical considerations regarding the treatment of potentially sentient AI entities, including rights and welfare (Forward-looking).</t>
   </si>
   <si>
-    <t>MIT AI Risk Rep: 7.5; Gartner: AI Ethics</t>
+    <t>MIT AI Risk Rep: 7.5; Gartner: AI Ethics; NIST AI RMF: GOVERN 1.2</t>
   </si>
   <si>
     <t>Sustainability</t>
@@ -592,7 +643,7 @@
     <t>The training and operation of AI models consume excessive energy/water, conflicting with corporate sustainability goals.</t>
   </si>
   <si>
-    <t>Gartner: AI Governance (Sustainable AI); Gartner: AI Engineering; MIT AI Risk Rep: 6.6; ISO/IEC 42001 (Sustainability B.5.5)</t>
+    <t>Gartner: AI Governance (Sustainable AI); Gartner: AI Engineering; MIT AI Risk Rep: 6.6; ISO/IEC 42001 (Sustainability B.5.5); NIST AI RMF: MEASURE 2.13, MAP 1.1</t>
   </si>
 </sst>
 </file>
@@ -606,7 +657,7 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="12"/>
@@ -614,20 +665,33 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="15"/>
+      <b val="1"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -637,34 +701,145 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,16 +858,19 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Blank">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -700,28 +878,28 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="A7A7A7"/>
+        <a:srgbClr val="5E5E5E"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="535353"/>
+        <a:srgbClr val="D5D5D5"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="00A2FF"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="16E7CF"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="61D836"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="FFD932"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="FF644E"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="FF42A1"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -730,7 +908,7 @@
         <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Blank">
       <a:majorFont>
         <a:latin typeface="Helvetica Neue"/>
         <a:ea typeface="Helvetica Neue"/>
@@ -742,7 +920,7 @@
         <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Sheets">
+    <a:fmtScheme name="Blank">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -880,23 +1058,20 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
+          <a:srgbClr val="000000"/>
         </a:solidFill>
         <a:ln w="12700" cap="flat">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:noFill/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -910,19 +1085,19 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="000000"/>
+              <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="Helvetica Neue Medium"/>
+            <a:ea typeface="Helvetica Neue Medium"/>
+            <a:cs typeface="Helvetica Neue Medium"/>
+            <a:sym typeface="Helvetica Neue Medium"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1163,10 +1338,10 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat">
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1443,11 +1618,11 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1470,10 +1645,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1718,952 +1893,1195 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A2:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="12.6719" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="137.672" style="1" customWidth="1"/>
+    <col min="5" max="5" width="123.672" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
+    <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="B2" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="C2" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="D2" t="s" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="E2" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="F2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="2">
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="B3" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="C3" t="s" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s" s="2">
+      <c r="D3" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="2">
+      <c r="E3" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="2">
+      <c r="F3" t="s" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s" s="2">
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s" s="9">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="2">
+      <c r="D4" t="s" s="9">
         <v>14</v>
       </c>
-      <c r="E4" t="s" s="2">
+      <c r="E4" t="s" s="9">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s" s="2">
+      <c r="F4" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="D5" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="E5" t="s" s="2">
+      <c r="E5" t="s" s="9">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="2">
+      <c r="F5" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s" s="9">
         <v>19</v>
       </c>
-      <c r="C6" t="s" s="2">
+      <c r="D6" t="s" s="9">
         <v>20</v>
       </c>
-      <c r="D6" t="s" s="2">
+      <c r="E6" t="s" s="9">
         <v>21</v>
       </c>
-      <c r="E6" t="s" s="2">
+      <c r="F6" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s" s="8">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s" s="2">
+      <c r="C7" t="s" s="9">
         <v>23</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="D7" t="s" s="9">
         <v>24</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="E7" t="s" s="9">
         <v>25</v>
       </c>
-      <c r="E7" t="s" s="2">
+      <c r="F7" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="8">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s" s="2">
+      <c r="C8" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="C8" t="s" s="2">
+      <c r="D8" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="D8" t="s" s="2">
+      <c r="E8" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="E8" t="s" s="2">
+      <c r="F8" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s" s="8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" t="s" s="2">
+      <c r="C9" t="s" s="9">
         <v>31</v>
       </c>
-      <c r="B9" t="s" s="2">
+      <c r="D9" t="s" s="9">
         <v>32</v>
       </c>
-      <c r="C9" t="s" s="2">
+      <c r="E9" t="s" s="9">
         <v>33</v>
       </c>
-      <c r="D9" t="s" s="2">
+      <c r="F9" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s" s="9">
         <v>34</v>
       </c>
-      <c r="E9" t="s" s="2">
+      <c r="D10" t="s" s="9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s" s="2">
+      <c r="E10" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="C10" t="s" s="2">
+      <c r="F10" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="D10" t="s" s="2">
+      <c r="B11" t="s" s="8">
         <v>38</v>
       </c>
-      <c r="E10" t="s" s="2">
+      <c r="C11" t="s" s="9">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s" s="2">
+      <c r="D11" t="s" s="9">
         <v>40</v>
       </c>
-      <c r="C11" t="s" s="2">
+      <c r="E11" t="s" s="9">
         <v>41</v>
       </c>
-      <c r="D11" t="s" s="2">
+      <c r="F11" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s" s="8">
         <v>42</v>
       </c>
-      <c r="E11" t="s" s="2">
+      <c r="C12" t="s" s="9">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s" s="2">
+      <c r="D12" t="s" s="9">
         <v>44</v>
       </c>
-      <c r="C12" t="s" s="2">
+      <c r="E12" t="s" s="9">
         <v>45</v>
       </c>
-      <c r="D12" t="s" s="2">
+      <c r="F12" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s" s="8">
         <v>46</v>
       </c>
-      <c r="E12" t="s" s="2">
+      <c r="C13" t="s" s="9">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" ht="13.65" customHeight="1">
-      <c r="A13" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="C13" t="s" s="2">
+      <c r="D13" t="s" s="9">
         <v>48</v>
       </c>
-      <c r="D13" t="s" s="2">
+      <c r="E13" t="s" s="9">
         <v>49</v>
       </c>
-      <c r="E13" t="s" s="2">
+      <c r="F13" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s" s="8">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" ht="13.65" customHeight="1">
-      <c r="A14" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s" s="2">
+      <c r="C14" t="s" s="9">
         <v>51</v>
       </c>
-      <c r="D14" t="s" s="2">
+      <c r="D14" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="E14" t="s" s="2">
+      <c r="E14" t="s" s="9">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" ht="13.65" customHeight="1">
-      <c r="A15" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s" s="2">
+      <c r="F14" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s" s="9">
         <v>54</v>
       </c>
-      <c r="D15" t="s" s="2">
+      <c r="D15" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="E15" t="s" s="2">
+      <c r="E15" t="s" s="9">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" ht="13.65" customHeight="1">
-      <c r="A16" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s" s="2">
+      <c r="F15" t="s" s="9">
         <v>57</v>
       </c>
-      <c r="D16" t="s" s="2">
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s" s="9">
         <v>58</v>
       </c>
-      <c r="E16" t="s" s="2">
+      <c r="D16" t="s" s="9">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" ht="13.65" customHeight="1">
-      <c r="A17" t="s" s="2">
+      <c r="E16" t="s" s="9">
         <v>60</v>
       </c>
-      <c r="B17" t="s" s="2">
+      <c r="F16" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s" s="9">
         <v>61</v>
       </c>
-      <c r="C17" t="s" s="2">
+      <c r="D17" t="s" s="9">
         <v>62</v>
       </c>
-      <c r="D17" t="s" s="2">
+      <c r="E17" t="s" s="9">
         <v>63</v>
       </c>
-      <c r="E17" t="s" s="2">
+      <c r="F17" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s" s="9">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" ht="13.65" customHeight="1">
-      <c r="A18" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="B18" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="C18" t="s" s="2">
+      <c r="D18" t="s" s="9">
         <v>65</v>
       </c>
-      <c r="D18" t="s" s="2">
+      <c r="E18" t="s" s="9">
         <v>66</v>
       </c>
-      <c r="E18" t="s" s="2">
+      <c r="F18" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" t="s" s="7">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" ht="13.65" customHeight="1">
-      <c r="A19" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="B19" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="C19" t="s" s="2">
+      <c r="B19" t="s" s="8">
         <v>68</v>
       </c>
-      <c r="D19" t="s" s="2">
+      <c r="C19" t="s" s="9">
         <v>69</v>
       </c>
-      <c r="E19" t="s" s="2">
+      <c r="D19" t="s" s="9">
         <v>70</v>
       </c>
-    </row>
-    <row r="20" ht="13.65" customHeight="1">
-      <c r="A20" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="C20" t="s" s="2">
+      <c r="E19" t="s" s="9">
         <v>71</v>
       </c>
-      <c r="D20" t="s" s="2">
+      <c r="F19" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s" s="9">
         <v>72</v>
       </c>
-      <c r="E20" t="s" s="2">
+      <c r="D20" t="s" s="9">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" ht="13.65" customHeight="1">
-      <c r="A21" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="B21" t="s" s="2">
+      <c r="E20" t="s" s="9">
         <v>74</v>
       </c>
-      <c r="C21" t="s" s="2">
+      <c r="F20" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="C21" t="s" s="9">
         <v>75</v>
       </c>
-      <c r="D21" t="s" s="2">
+      <c r="D21" t="s" s="9">
         <v>76</v>
       </c>
-      <c r="E21" t="s" s="2">
+      <c r="E21" t="s" s="9">
         <v>77</v>
       </c>
-    </row>
-    <row r="22" ht="13.65" customHeight="1">
-      <c r="A22" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="C22" t="s" s="2">
+      <c r="F21" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s" s="9">
         <v>78</v>
       </c>
-      <c r="D22" t="s" s="2">
+      <c r="D22" t="s" s="9">
         <v>79</v>
       </c>
-      <c r="E22" t="s" s="2">
+      <c r="E22" t="s" s="9">
         <v>80</v>
       </c>
-    </row>
-    <row r="23" ht="13.65" customHeight="1">
-      <c r="A23" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="B23" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="C23" t="s" s="2">
+      <c r="F22" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s" s="8">
         <v>81</v>
       </c>
-      <c r="D23" t="s" s="2">
+      <c r="C23" t="s" s="9">
         <v>82</v>
       </c>
-      <c r="E23" t="s" s="2">
+      <c r="D23" t="s" s="9">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" ht="13.65" customHeight="1">
-      <c r="A24" t="s" s="2">
+      <c r="E23" t="s" s="9">
         <v>84</v>
       </c>
-      <c r="B24" t="s" s="2">
+      <c r="F23" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s" s="9">
         <v>85</v>
       </c>
-      <c r="C24" t="s" s="2">
+      <c r="D24" t="s" s="9">
         <v>86</v>
       </c>
-      <c r="D24" t="s" s="2">
+      <c r="E24" t="s" s="9">
         <v>87</v>
       </c>
-      <c r="E24" t="s" s="2">
+      <c r="F24" t="s" s="9">
         <v>88</v>
       </c>
     </row>
-    <row r="25" ht="13.65" customHeight="1">
-      <c r="A25" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="B25" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="C25" t="s" s="2">
+    <row r="25" ht="20.05" customHeight="1">
+      <c r="A25" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="C25" t="s" s="9">
         <v>89</v>
       </c>
-      <c r="D25" t="s" s="2">
+      <c r="D25" t="s" s="9">
         <v>90</v>
       </c>
-      <c r="E25" t="s" s="2">
+      <c r="E25" t="s" s="9">
         <v>91</v>
       </c>
-    </row>
-    <row r="26" ht="13.65" customHeight="1">
-      <c r="A26" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="B26" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="C26" t="s" s="2">
+      <c r="F25" t="s" s="9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" ht="20.05" customHeight="1">
+      <c r="A26" t="s" s="7">
         <v>92</v>
       </c>
-      <c r="D26" t="s" s="2">
+      <c r="B26" t="s" s="8">
         <v>93</v>
       </c>
-      <c r="E26" t="s" s="2">
+      <c r="C26" t="s" s="9">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" ht="13.65" customHeight="1">
-      <c r="A27" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="B27" t="s" s="2">
+      <c r="D26" t="s" s="9">
         <v>95</v>
       </c>
-      <c r="C27" t="s" s="2">
+      <c r="E26" t="s" s="9">
         <v>96</v>
       </c>
-      <c r="D27" t="s" s="2">
+      <c r="F26" t="s" s="9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
+      <c r="A27" t="s" s="7">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s" s="8">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s" s="9">
         <v>97</v>
       </c>
-      <c r="E27" t="s" s="2">
+      <c r="D27" t="s" s="9">
         <v>98</v>
       </c>
-    </row>
-    <row r="28" ht="13.65" customHeight="1">
-      <c r="A28" t="s" s="2">
+      <c r="E27" t="s" s="9">
         <v>99</v>
       </c>
-      <c r="B28" t="s" s="2">
+      <c r="F27" t="s" s="9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" ht="20.05" customHeight="1">
+      <c r="A28" t="s" s="7">
+        <v>92</v>
+      </c>
+      <c r="B28" t="s" s="8">
+        <v>93</v>
+      </c>
+      <c r="C28" t="s" s="9">
         <v>100</v>
       </c>
-      <c r="C28" t="s" s="2">
+      <c r="D28" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="D28" t="s" s="2">
+      <c r="E28" t="s" s="9">
         <v>102</v>
       </c>
-      <c r="E28" t="s" s="2">
+      <c r="F28" t="s" s="9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" ht="20.05" customHeight="1">
+      <c r="A29" t="s" s="7">
+        <v>92</v>
+      </c>
+      <c r="B29" t="s" s="8">
         <v>103</v>
       </c>
-    </row>
-    <row r="29" ht="13.65" customHeight="1">
-      <c r="A29" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B29" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="C29" t="s" s="2">
+      <c r="C29" t="s" s="9">
         <v>104</v>
       </c>
-      <c r="D29" t="s" s="2">
+      <c r="D29" t="s" s="9">
         <v>105</v>
       </c>
-      <c r="E29" t="s" s="2">
+      <c r="E29" t="s" s="9">
         <v>106</v>
       </c>
-    </row>
-    <row r="30" ht="13.65" customHeight="1">
-      <c r="A30" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B30" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="C30" t="s" s="2">
+      <c r="F29" t="s" s="9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" ht="20.05" customHeight="1">
+      <c r="A30" t="s" s="7">
         <v>107</v>
       </c>
-      <c r="D30" t="s" s="2">
+      <c r="B30" t="s" s="8">
         <v>108</v>
       </c>
-      <c r="E30" t="s" s="2">
+      <c r="C30" t="s" s="9">
         <v>109</v>
       </c>
-    </row>
-    <row r="31" ht="13.65" customHeight="1">
-      <c r="A31" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B31" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="C31" t="s" s="2">
+      <c r="D30" t="s" s="9">
         <v>110</v>
       </c>
-      <c r="D31" t="s" s="2">
+      <c r="E30" t="s" s="9">
         <v>111</v>
       </c>
-      <c r="E31" t="s" s="2">
+      <c r="F30" t="s" s="9">
         <v>112</v>
       </c>
     </row>
-    <row r="32" ht="13.65" customHeight="1">
-      <c r="A32" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B32" t="s" s="2">
+    <row r="31" ht="20.05" customHeight="1">
+      <c r="A31" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B31" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="C31" t="s" s="9">
         <v>113</v>
       </c>
-      <c r="C32" t="s" s="2">
+      <c r="D31" t="s" s="9">
         <v>114</v>
       </c>
-      <c r="D32" t="s" s="2">
+      <c r="E31" t="s" s="9">
         <v>115</v>
       </c>
-      <c r="E32" t="s" s="2">
+      <c r="F31" t="s" s="9">
         <v>116</v>
       </c>
     </row>
-    <row r="33" ht="13.65" customHeight="1">
-      <c r="A33" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B33" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="C33" t="s" s="2">
+    <row r="32" ht="20.05" customHeight="1">
+      <c r="A32" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B32" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="C32" t="s" s="9">
         <v>117</v>
       </c>
-      <c r="D33" t="s" s="2">
+      <c r="D32" t="s" s="9">
         <v>118</v>
       </c>
-      <c r="E33" t="s" s="2">
+      <c r="E32" t="s" s="9">
         <v>119</v>
       </c>
-    </row>
-    <row r="34" ht="13.65" customHeight="1">
-      <c r="A34" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B34" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="C34" t="s" s="2">
+      <c r="F32" t="s" s="9">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" ht="20.05" customHeight="1">
+      <c r="A33" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="C33" t="s" s="9">
         <v>120</v>
       </c>
-      <c r="D34" t="s" s="2">
+      <c r="D33" t="s" s="9">
         <v>121</v>
       </c>
-      <c r="E34" t="s" s="2">
+      <c r="E33" t="s" s="9">
         <v>122</v>
       </c>
-    </row>
-    <row r="35" ht="13.65" customHeight="1">
-      <c r="A35" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B35" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="C35" t="s" s="2">
+      <c r="F33" t="s" s="9">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" ht="20.05" customHeight="1">
+      <c r="A34" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s" s="8">
         <v>123</v>
       </c>
-      <c r="D35" t="s" s="2">
+      <c r="C34" t="s" s="9">
         <v>124</v>
       </c>
-      <c r="E35" t="s" s="2">
+      <c r="D34" t="s" s="9">
         <v>125</v>
       </c>
-    </row>
-    <row r="36" ht="13.65" customHeight="1">
-      <c r="A36" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B36" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="C36" t="s" s="2">
+      <c r="E34" t="s" s="9">
         <v>126</v>
       </c>
-      <c r="D36" t="s" s="2">
+      <c r="F34" t="s" s="9">
         <v>127</v>
       </c>
-      <c r="E36" t="s" s="2">
+    </row>
+    <row r="35" ht="20.05" customHeight="1">
+      <c r="A35" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B35" t="s" s="8">
+        <v>123</v>
+      </c>
+      <c r="C35" t="s" s="9">
         <v>128</v>
       </c>
-    </row>
-    <row r="37" ht="13.65" customHeight="1">
-      <c r="A37" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B37" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="C37" t="s" s="2">
+      <c r="D35" t="s" s="9">
         <v>129</v>
       </c>
-      <c r="D37" t="s" s="2">
+      <c r="E35" t="s" s="9">
         <v>130</v>
       </c>
-      <c r="E37" t="s" s="2">
+      <c r="F35" t="s" s="9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" ht="20.05" customHeight="1">
+      <c r="A36" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s" s="8">
+        <v>123</v>
+      </c>
+      <c r="C36" t="s" s="9">
         <v>131</v>
       </c>
-    </row>
-    <row r="38" ht="13.65" customHeight="1">
-      <c r="A38" t="s" s="2">
+      <c r="D36" t="s" s="9">
         <v>132</v>
       </c>
-      <c r="B38" t="s" s="2">
+      <c r="E36" t="s" s="9">
         <v>133</v>
       </c>
-      <c r="C38" t="s" s="2">
+      <c r="F36" t="s" s="9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" ht="20.05" customHeight="1">
+      <c r="A37" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B37" t="s" s="8">
+        <v>123</v>
+      </c>
+      <c r="C37" t="s" s="9">
         <v>134</v>
       </c>
-      <c r="D38" t="s" s="2">
+      <c r="D37" t="s" s="9">
         <v>135</v>
       </c>
-      <c r="E38" t="s" s="2">
+      <c r="E37" t="s" s="9">
         <v>136</v>
       </c>
-    </row>
-    <row r="39" ht="13.65" customHeight="1">
-      <c r="A39" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="B39" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="C39" t="s" s="2">
+      <c r="F37" t="s" s="9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" ht="20.05" customHeight="1">
+      <c r="A38" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B38" t="s" s="8">
+        <v>123</v>
+      </c>
+      <c r="C38" t="s" s="9">
         <v>137</v>
       </c>
-      <c r="D39" t="s" s="2">
+      <c r="D38" t="s" s="9">
         <v>138</v>
       </c>
-      <c r="E39" t="s" s="2">
+      <c r="E38" t="s" s="9">
         <v>139</v>
       </c>
-    </row>
-    <row r="40" ht="13.65" customHeight="1">
-      <c r="A40" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="B40" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="C40" t="s" s="2">
+      <c r="F38" t="s" s="9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" ht="20.05" customHeight="1">
+      <c r="A39" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B39" t="s" s="8">
+        <v>123</v>
+      </c>
+      <c r="C39" t="s" s="9">
         <v>140</v>
       </c>
-      <c r="D40" t="s" s="2">
+      <c r="D39" t="s" s="9">
         <v>141</v>
       </c>
-      <c r="E40" t="s" s="2">
+      <c r="E39" t="s" s="9">
         <v>142</v>
       </c>
-    </row>
-    <row r="41" ht="13.65" customHeight="1">
-      <c r="A41" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="B41" t="s" s="2">
+      <c r="F39" t="s" s="9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" ht="20.05" customHeight="1">
+      <c r="A40" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B40" t="s" s="8">
+        <v>123</v>
+      </c>
+      <c r="C40" t="s" s="9">
         <v>143</v>
       </c>
-      <c r="C41" t="s" s="2">
+      <c r="D40" t="s" s="9">
         <v>144</v>
       </c>
-      <c r="D41" t="s" s="2">
+      <c r="E40" t="s" s="9">
         <v>145</v>
       </c>
-      <c r="E41" t="s" s="2">
+      <c r="F40" t="s" s="9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" ht="20.05" customHeight="1">
+      <c r="A41" t="s" s="7">
         <v>146</v>
       </c>
-    </row>
-    <row r="42" ht="13.65" customHeight="1">
-      <c r="A42" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="B42" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="C42" t="s" s="2">
+      <c r="B41" t="s" s="8">
         <v>147</v>
       </c>
-      <c r="D42" t="s" s="2">
+      <c r="C41" t="s" s="9">
         <v>148</v>
       </c>
-      <c r="E42" t="s" s="2">
+      <c r="D41" t="s" s="9">
         <v>149</v>
       </c>
-    </row>
-    <row r="43" ht="13.65" customHeight="1">
-      <c r="A43" t="s" s="2">
+      <c r="E41" t="s" s="9">
         <v>150</v>
       </c>
-      <c r="B43" t="s" s="2">
+      <c r="F41" t="s" s="9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" ht="20.05" customHeight="1">
+      <c r="A42" t="s" s="7">
+        <v>146</v>
+      </c>
+      <c r="B42" t="s" s="8">
+        <v>147</v>
+      </c>
+      <c r="C42" t="s" s="9">
         <v>151</v>
       </c>
-      <c r="C43" t="s" s="2">
+      <c r="D42" t="s" s="9">
         <v>152</v>
       </c>
-      <c r="D43" t="s" s="2">
+      <c r="E42" t="s" s="9">
         <v>153</v>
       </c>
-      <c r="E43" t="s" s="2">
+      <c r="F42" t="s" s="9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" ht="20.05" customHeight="1">
+      <c r="A43" t="s" s="7">
+        <v>146</v>
+      </c>
+      <c r="B43" t="s" s="8">
+        <v>147</v>
+      </c>
+      <c r="C43" t="s" s="9">
         <v>154</v>
       </c>
-    </row>
-    <row r="44" ht="13.65" customHeight="1">
-      <c r="A44" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B44" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="C44" t="s" s="2">
+      <c r="D43" t="s" s="9">
         <v>155</v>
       </c>
-      <c r="D44" t="s" s="2">
+      <c r="E43" t="s" s="9">
         <v>156</v>
       </c>
-      <c r="E44" t="s" s="2">
+      <c r="F43" t="s" s="9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" ht="20.05" customHeight="1">
+      <c r="A44" t="s" s="7">
+        <v>146</v>
+      </c>
+      <c r="B44" t="s" s="8">
         <v>157</v>
       </c>
-    </row>
-    <row r="45" ht="13.65" customHeight="1">
-      <c r="A45" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B45" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="C45" t="s" s="2">
+      <c r="C44" t="s" s="9">
         <v>158</v>
       </c>
-      <c r="D45" t="s" s="2">
+      <c r="D44" t="s" s="9">
         <v>159</v>
       </c>
-      <c r="E45" t="s" s="2">
+      <c r="E44" t="s" s="9">
         <v>160</v>
       </c>
-    </row>
-    <row r="46" ht="13.65" customHeight="1">
-      <c r="A46" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B46" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="C46" t="s" s="2">
+      <c r="F44" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" ht="20.05" customHeight="1">
+      <c r="A45" t="s" s="7">
+        <v>146</v>
+      </c>
+      <c r="B45" t="s" s="8">
+        <v>157</v>
+      </c>
+      <c r="C45" t="s" s="9">
         <v>161</v>
       </c>
-      <c r="D46" t="s" s="2">
+      <c r="D45" t="s" s="9">
         <v>162</v>
       </c>
-      <c r="E46" t="s" s="2">
+      <c r="E45" t="s" s="9">
         <v>163</v>
       </c>
-    </row>
-    <row r="47" ht="13.65" customHeight="1">
-      <c r="A47" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B47" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="C47" t="s" s="2">
+      <c r="F45" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" ht="20.05" customHeight="1">
+      <c r="A46" t="s" s="7">
         <v>164</v>
       </c>
-      <c r="D47" t="s" s="2">
+      <c r="B46" t="s" s="8">
         <v>165</v>
       </c>
-      <c r="E47" t="s" s="2">
+      <c r="C46" t="s" s="9">
         <v>166</v>
       </c>
-    </row>
-    <row r="48" ht="13.65" customHeight="1">
-      <c r="A48" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B48" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="C48" t="s" s="2">
+      <c r="D46" t="s" s="9">
         <v>167</v>
       </c>
-      <c r="D48" t="s" s="2">
+      <c r="E46" t="s" s="9">
         <v>168</v>
       </c>
-      <c r="E48" t="s" s="2">
+      <c r="F46" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" ht="20.05" customHeight="1">
+      <c r="A47" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B47" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="C47" t="s" s="9">
         <v>169</v>
       </c>
-    </row>
-    <row r="49" ht="13.65" customHeight="1">
-      <c r="A49" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B49" t="s" s="2">
+      <c r="D47" t="s" s="9">
         <v>170</v>
       </c>
-      <c r="C49" t="s" s="2">
+      <c r="E47" t="s" s="9">
         <v>171</v>
       </c>
-      <c r="D49" t="s" s="2">
+      <c r="F47" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" ht="20.05" customHeight="1">
+      <c r="A48" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B48" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="C48" t="s" s="9">
         <v>172</v>
       </c>
-      <c r="E49" t="s" s="2">
+      <c r="D48" t="s" s="9">
         <v>173</v>
       </c>
-    </row>
-    <row r="50" ht="13.65" customHeight="1">
-      <c r="A50" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B50" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="C50" t="s" s="2">
+      <c r="E48" t="s" s="9">
         <v>174</v>
       </c>
-      <c r="D50" t="s" s="2">
+      <c r="F48" t="s" s="9">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" ht="20.05" customHeight="1">
+      <c r="A49" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B49" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="C49" t="s" s="9">
         <v>175</v>
       </c>
-      <c r="E50" t="s" s="2">
+      <c r="D49" t="s" s="9">
         <v>176</v>
       </c>
-    </row>
-    <row r="51" ht="13.65" customHeight="1">
-      <c r="A51" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B51" t="s" s="2">
+      <c r="E49" t="s" s="9">
         <v>177</v>
       </c>
-      <c r="C51" t="s" s="2">
+      <c r="F49" t="s" s="9">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" ht="20.05" customHeight="1">
+      <c r="A50" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B50" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="C50" t="s" s="9">
         <v>178</v>
       </c>
-      <c r="D51" t="s" s="2">
+      <c r="D50" t="s" s="9">
         <v>179</v>
       </c>
-      <c r="E51" t="s" s="2">
+      <c r="E50" t="s" s="9">
         <v>180</v>
       </c>
-    </row>
-    <row r="52" ht="13.65" customHeight="1">
-      <c r="A52" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B52" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="C52" t="s" s="2">
+      <c r="F50" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" ht="20.05" customHeight="1">
+      <c r="A51" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B51" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="C51" t="s" s="9">
         <v>181</v>
       </c>
-      <c r="D52" t="s" s="2">
+      <c r="D51" t="s" s="9">
         <v>182</v>
       </c>
-      <c r="E52" t="s" s="2">
+      <c r="E51" t="s" s="9">
         <v>183</v>
       </c>
-    </row>
-    <row r="53" ht="13.65" customHeight="1">
-      <c r="A53" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B53" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="C53" t="s" s="2">
+      <c r="F51" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" ht="20.05" customHeight="1">
+      <c r="A52" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B52" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="C52" t="s" s="9">
         <v>184</v>
       </c>
-      <c r="D53" t="s" s="2">
+      <c r="D52" t="s" s="9">
         <v>185</v>
       </c>
-      <c r="E53" t="s" s="2">
+      <c r="E52" t="s" s="9">
         <v>186</v>
       </c>
-    </row>
-    <row r="54" ht="13.65" customHeight="1">
-      <c r="A54" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B54" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="C54" t="s" s="2">
+      <c r="F52" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" ht="20.05" customHeight="1">
+      <c r="A53" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B53" t="s" s="8">
         <v>187</v>
       </c>
-      <c r="D54" t="s" s="2">
+      <c r="C53" t="s" s="9">
         <v>188</v>
       </c>
-      <c r="E54" t="s" s="2">
+      <c r="D53" t="s" s="9">
         <v>189</v>
       </c>
-    </row>
-    <row r="55" ht="13.65" customHeight="1">
-      <c r="A55" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="B55" t="s" s="2">
+      <c r="E53" t="s" s="9">
         <v>190</v>
       </c>
-      <c r="C55" t="s" s="2">
+      <c r="F53" t="s" s="9">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" ht="20.05" customHeight="1">
+      <c r="A54" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B54" t="s" s="8">
+        <v>187</v>
+      </c>
+      <c r="C54" t="s" s="9">
         <v>191</v>
       </c>
-      <c r="D55" t="s" s="2">
+      <c r="D54" t="s" s="9">
         <v>192</v>
       </c>
-      <c r="E55" t="s" s="2">
+      <c r="E54" t="s" s="9">
         <v>193</v>
       </c>
+      <c r="F54" t="s" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" ht="20.05" customHeight="1">
+      <c r="A55" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B55" t="s" s="8">
+        <v>194</v>
+      </c>
+      <c r="C55" t="s" s="9">
+        <v>195</v>
+      </c>
+      <c r="D55" t="s" s="9">
+        <v>196</v>
+      </c>
+      <c r="E55" t="s" s="9">
+        <v>197</v>
+      </c>
+      <c r="F55" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" ht="20.05" customHeight="1">
+      <c r="A56" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B56" t="s" s="8">
+        <v>194</v>
+      </c>
+      <c r="C56" t="s" s="9">
+        <v>198</v>
+      </c>
+      <c r="D56" t="s" s="9">
+        <v>199</v>
+      </c>
+      <c r="E56" t="s" s="9">
+        <v>200</v>
+      </c>
+      <c r="F56" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" ht="20.05" customHeight="1">
+      <c r="A57" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B57" t="s" s="8">
+        <v>194</v>
+      </c>
+      <c r="C57" t="s" s="9">
+        <v>201</v>
+      </c>
+      <c r="D57" t="s" s="9">
+        <v>202</v>
+      </c>
+      <c r="E57" t="s" s="9">
+        <v>203</v>
+      </c>
+      <c r="F57" t="s" s="9">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" ht="20.05" customHeight="1">
+      <c r="A58" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B58" t="s" s="8">
+        <v>194</v>
+      </c>
+      <c r="C58" t="s" s="9">
+        <v>204</v>
+      </c>
+      <c r="D58" t="s" s="9">
+        <v>205</v>
+      </c>
+      <c r="E58" t="s" s="9">
+        <v>206</v>
+      </c>
+      <c r="F58" t="s" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" ht="20.05" customHeight="1">
+      <c r="A59" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="B59" t="s" s="8">
+        <v>207</v>
+      </c>
+      <c r="C59" t="s" s="9">
+        <v>208</v>
+      </c>
+      <c r="D59" t="s" s="9">
+        <v>209</v>
+      </c>
+      <c r="E59" t="s" s="9">
+        <v>210</v>
+      </c>
+      <c r="F59" t="s" s="9">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
Refine details modal: Rename NIST Stage to AI Lifecycle Stage and reposition above Risk Name
</commit_message>
<xml_diff>
--- a/data/risk_matrix.xlsx
+++ b/data/risk_matrix.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="211">
-  <si>
-    <t>risk_matrix v2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="212">
   <si>
     <t>Process Name</t>
   </si>
@@ -34,6 +31,9 @@
     <t>NIST AI Lifecycle Stage</t>
   </si>
   <si>
+    <t>URL Sources</t>
+  </si>
+  <si>
     <t>1. AI Strategy &amp; Value Mgmt.</t>
   </si>
   <si>
@@ -49,7 +49,182 @@
     <t>Gartner: AI Roadmap; Gartner: AI Strategy; ISO/IEC 42001 (Context of Org); NIST AI RMF: MAP 1.1, MAP 1.2</t>
   </si>
   <si>
-    <t>Plan &amp; Design</t>
+    <t>1. Plan &amp; Design</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Gartner - AI Roadmap Toolkit (public) | </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.gartner.com/en/chief-information-officer/research/ai-maturity-model-toolkit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> || 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Gartner - AI Strategy Reference Guide (internal) | </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.gartner.com/document-reader/document/5938007?ref=pubsite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> || 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Gartner - AI Strategy for Business (public) | </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.gartner.com/en/articles/ai-strategy-for-business</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> || 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Gartner - The Pillars of a Successful Artificial Intelligence Strategy (internal) | </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.gartner.com/document-reader/document/5373763?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> || 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Gartner - Reference Guide for AI Strategy (internal) | </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.gartner.com/document-reader/document/6676234?ref=pubsite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> || 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">ISO/IEC 42001:2023 - Information technology — Artificial intelligence — Management syste (public) | </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.iso.org/standard/42001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> || 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">NIST - AI Risk Management Framework (public) | </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.nist.gov/itl/ai-risk-management-framework</t>
+    </r>
   </si>
   <si>
     <t>Competitive Race Risk</t>
@@ -184,7 +359,7 @@
     <t>OWASP LLM Top 10: LLM09; MIT AI Risk Rep: 5.2; Gartner: AI People &amp; Culture; NIST AI RMF: MAP 1.1, MANAGE 3.2</t>
   </si>
   <si>
-    <t>Use</t>
+    <t>6. Use</t>
   </si>
   <si>
     <t>User Resistance &amp; Adoption Failure</t>
@@ -277,7 +452,7 @@
     <t>OWASP LLM Top 10: LLM05; OWASP ML Top 10: ML06; ISO/IEC 42001 (Suppliers A.10.3); NIST AI RMF: MANAGE 1.3, MAP 2.3</t>
   </si>
   <si>
-    <t>Collect &amp; Process Data</t>
+    <t>2. Collect &amp; Process Data</t>
   </si>
   <si>
     <t>Intellectual Property Infringement</t>
@@ -349,7 +524,7 @@
     <t>Gartner: AI Roadmap; Gartner: AI Engineering; NIST AI RMF: MANAGE 2.2</t>
   </si>
   <si>
-    <t>Build</t>
+    <t>3. Build (&amp; Use Model)</t>
   </si>
   <si>
     <t>Inadequate Verification &amp; Validation</t>
@@ -361,7 +536,7 @@
     <t>ISO/IEC 5338 (Verification); ISO/IEC 42001 (Control A.6.2.4); MITRE: Test &amp; Evaluation; NIST AI RMF: MEASURE 1.1, MEASURE 2.6</t>
   </si>
   <si>
-    <t>Verify &amp; Validate</t>
+    <t>4. Verify &amp; Validate</t>
   </si>
   <si>
     <t>Insecure Output Handling</t>
@@ -394,7 +569,7 @@
     <t>Gartner: AI Engineering; MITRE: Solution Monitoring; OWASP ML Top 10: ML08; NIST AI RMF: MANAGE 4.2, MEASURE 2.12</t>
   </si>
   <si>
-    <t>Operate &amp; Monitor</t>
+    <t>5. Operate &amp; Monitor</t>
   </si>
   <si>
     <t>Continuous Validation Failure</t>
@@ -653,7 +828,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -665,13 +840,24 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="14"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -690,8 +876,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -764,6 +956,21 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -810,35 +1017,41 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -862,6 +1075,8 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -878,10 +1093,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -1058,11 +1273,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1071,7 +1289,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1085,19 +1303,19 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1336,12 +1554,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1622,7 +1840,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1893,7 +2111,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:F59"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1904,1184 +2122,1237 @@
     <col min="3" max="3" width="38.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="137.672" style="1" customWidth="1"/>
     <col min="5" max="5" width="123.672" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.8516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="107.172" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="3">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="3">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B2" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C2" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D2" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="E2" t="s" s="5">
         <v>11</v>
+      </c>
+      <c r="F2" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s" s="10">
+        <v>16</v>
       </c>
       <c r="F3" t="s" s="6">
         <v>12</v>
       </c>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="A4" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="C4" t="s" s="9">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s" s="9">
+      <c r="C4" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s" s="6">
         <v>12</v>
       </c>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="A5" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="B5" t="s" s="8">
+      <c r="B5" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="C5" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s" s="9">
+      <c r="C5" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s" s="6">
         <v>12</v>
       </c>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="7">
+      <c r="A6" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="B6" t="s" s="8">
+      <c r="B6" t="s" s="9">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="10">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s" s="10">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s" s="10">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s" s="10">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="C6" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s" s="9">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s" s="9">
+      <c r="C9" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s" s="10">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s" s="6">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s" s="8">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s" s="9">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s" s="9">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s" s="9">
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s" s="9">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s" s="10">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s" s="10">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s" s="6">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s" s="8">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s" s="9">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s" s="9">
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s" s="9">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s" s="10">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s" s="10">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s" s="10">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s" s="6">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s" s="9">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s" s="9">
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s" s="9">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s" s="10">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s" s="10">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s" s="10">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s" s="6">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s" s="9">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s" s="9">
-        <v>35</v>
-      </c>
-      <c r="E10" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s" s="9">
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s" s="10">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s" s="10">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s" s="10">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s" s="8">
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" t="s" s="8">
         <v>38</v>
       </c>
-      <c r="C11" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s" s="9">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s" s="9">
-        <v>41</v>
-      </c>
-      <c r="F11" t="s" s="9">
+      <c r="B14" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s" s="10">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s" s="10">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s" s="10">
+        <v>57</v>
+      </c>
+      <c r="F14" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s" s="10">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s" s="10">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s" s="10">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s" s="10">
+        <v>62</v>
+      </c>
+      <c r="D16" t="s" s="10">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s" s="10">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s" s="10">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s" s="10">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s" s="10">
+        <v>67</v>
+      </c>
+      <c r="F17" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s" s="9">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s" s="10">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="E18" t="s" s="10">
+        <v>72</v>
+      </c>
+      <c r="F18" t="s" s="11">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B12" t="s" s="8">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="E12" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="F12" t="s" s="9">
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s" s="9">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s" s="10">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s" s="10">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s" s="10">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s" s="6">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s" s="8">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s" s="9">
-        <v>47</v>
-      </c>
-      <c r="D13" t="s" s="9">
-        <v>48</v>
-      </c>
-      <c r="E13" t="s" s="9">
-        <v>49</v>
-      </c>
-      <c r="F13" t="s" s="9">
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s" s="9">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s" s="10">
+        <v>76</v>
+      </c>
+      <c r="D20" t="s" s="10">
+        <v>77</v>
+      </c>
+      <c r="E20" t="s" s="10">
+        <v>78</v>
+      </c>
+      <c r="F20" t="s" s="6">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="C14" t="s" s="9">
-        <v>51</v>
-      </c>
-      <c r="D14" t="s" s="9">
-        <v>52</v>
-      </c>
-      <c r="E14" t="s" s="9">
-        <v>53</v>
-      </c>
-      <c r="F14" t="s" s="9">
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s" s="9">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s" s="10">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s" s="10">
+        <v>80</v>
+      </c>
+      <c r="E21" t="s" s="10">
+        <v>81</v>
+      </c>
+      <c r="F21" t="s" s="6">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="C15" t="s" s="9">
-        <v>54</v>
-      </c>
-      <c r="D15" t="s" s="9">
-        <v>55</v>
-      </c>
-      <c r="E15" t="s" s="9">
-        <v>56</v>
-      </c>
-      <c r="F15" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="C16" t="s" s="9">
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s" s="9">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s" s="10">
+        <v>83</v>
+      </c>
+      <c r="D22" t="s" s="10">
+        <v>84</v>
+      </c>
+      <c r="E22" t="s" s="10">
+        <v>85</v>
+      </c>
+      <c r="F22" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s" s="9">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s" s="10">
+        <v>86</v>
+      </c>
+      <c r="D23" t="s" s="10">
+        <v>87</v>
+      </c>
+      <c r="E23" t="s" s="10">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s" s="10">
+        <v>89</v>
+      </c>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s" s="9">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s" s="10">
+        <v>90</v>
+      </c>
+      <c r="D24" t="s" s="10">
+        <v>91</v>
+      </c>
+      <c r="E24" t="s" s="10">
+        <v>92</v>
+      </c>
+      <c r="F24" t="s" s="10">
+        <v>89</v>
+      </c>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" ht="20.05" customHeight="1">
+      <c r="A25" t="s" s="8">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s" s="9">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s" s="10">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s" s="10">
+        <v>96</v>
+      </c>
+      <c r="E25" t="s" s="10">
+        <v>97</v>
+      </c>
+      <c r="F25" t="s" s="10">
+        <v>89</v>
+      </c>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" ht="20.05" customHeight="1">
+      <c r="A26" t="s" s="8">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s" s="9">
+        <v>94</v>
+      </c>
+      <c r="C26" t="s" s="10">
+        <v>98</v>
+      </c>
+      <c r="D26" t="s" s="10">
+        <v>99</v>
+      </c>
+      <c r="E26" t="s" s="10">
+        <v>100</v>
+      </c>
+      <c r="F26" t="s" s="10">
+        <v>89</v>
+      </c>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
+      <c r="A27" t="s" s="8">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s" s="9">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s" s="10">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s" s="10">
+        <v>102</v>
+      </c>
+      <c r="E27" t="s" s="10">
+        <v>103</v>
+      </c>
+      <c r="F27" t="s" s="10">
+        <v>89</v>
+      </c>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" ht="20.05" customHeight="1">
+      <c r="A28" t="s" s="8">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s" s="9">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s" s="10">
+        <v>105</v>
+      </c>
+      <c r="D28" t="s" s="10">
+        <v>106</v>
+      </c>
+      <c r="E28" t="s" s="10">
+        <v>107</v>
+      </c>
+      <c r="F28" t="s" s="10">
+        <v>89</v>
+      </c>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" ht="20.05" customHeight="1">
+      <c r="A29" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s" s="9">
+        <v>109</v>
+      </c>
+      <c r="C29" t="s" s="10">
+        <v>110</v>
+      </c>
+      <c r="D29" t="s" s="10">
+        <v>111</v>
+      </c>
+      <c r="E29" t="s" s="10">
+        <v>112</v>
+      </c>
+      <c r="F29" t="s" s="10">
+        <v>113</v>
+      </c>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" ht="20.05" customHeight="1">
+      <c r="A30" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B30" t="s" s="9">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s" s="10">
+        <v>114</v>
+      </c>
+      <c r="D30" t="s" s="10">
+        <v>115</v>
+      </c>
+      <c r="E30" t="s" s="10">
+        <v>116</v>
+      </c>
+      <c r="F30" t="s" s="10">
+        <v>117</v>
+      </c>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" ht="20.05" customHeight="1">
+      <c r="A31" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B31" t="s" s="9">
+        <v>109</v>
+      </c>
+      <c r="C31" t="s" s="10">
+        <v>118</v>
+      </c>
+      <c r="D31" t="s" s="10">
+        <v>119</v>
+      </c>
+      <c r="E31" t="s" s="10">
+        <v>120</v>
+      </c>
+      <c r="F31" t="s" s="10">
+        <v>113</v>
+      </c>
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" ht="20.05" customHeight="1">
+      <c r="A32" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B32" t="s" s="9">
+        <v>109</v>
+      </c>
+      <c r="C32" t="s" s="10">
+        <v>121</v>
+      </c>
+      <c r="D32" t="s" s="10">
+        <v>122</v>
+      </c>
+      <c r="E32" t="s" s="10">
+        <v>123</v>
+      </c>
+      <c r="F32" t="s" s="10">
+        <v>113</v>
+      </c>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" ht="20.05" customHeight="1">
+      <c r="A33" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B33" t="s" s="9">
+        <v>124</v>
+      </c>
+      <c r="C33" t="s" s="10">
+        <v>125</v>
+      </c>
+      <c r="D33" t="s" s="10">
+        <v>126</v>
+      </c>
+      <c r="E33" t="s" s="10">
+        <v>127</v>
+      </c>
+      <c r="F33" t="s" s="10">
+        <v>128</v>
+      </c>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" ht="20.05" customHeight="1">
+      <c r="A34" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B34" t="s" s="9">
+        <v>124</v>
+      </c>
+      <c r="C34" t="s" s="10">
+        <v>129</v>
+      </c>
+      <c r="D34" t="s" s="10">
+        <v>130</v>
+      </c>
+      <c r="E34" t="s" s="10">
+        <v>131</v>
+      </c>
+      <c r="F34" t="s" s="10">
+        <v>128</v>
+      </c>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" ht="20.05" customHeight="1">
+      <c r="A35" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s" s="9">
+        <v>124</v>
+      </c>
+      <c r="C35" t="s" s="10">
+        <v>132</v>
+      </c>
+      <c r="D35" t="s" s="10">
+        <v>133</v>
+      </c>
+      <c r="E35" t="s" s="10">
+        <v>134</v>
+      </c>
+      <c r="F35" t="s" s="10">
+        <v>128</v>
+      </c>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" ht="20.05" customHeight="1">
+      <c r="A36" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B36" t="s" s="9">
+        <v>124</v>
+      </c>
+      <c r="C36" t="s" s="10">
+        <v>135</v>
+      </c>
+      <c r="D36" t="s" s="10">
+        <v>136</v>
+      </c>
+      <c r="E36" t="s" s="10">
+        <v>137</v>
+      </c>
+      <c r="F36" t="s" s="10">
+        <v>128</v>
+      </c>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" ht="20.05" customHeight="1">
+      <c r="A37" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B37" t="s" s="9">
+        <v>124</v>
+      </c>
+      <c r="C37" t="s" s="10">
+        <v>138</v>
+      </c>
+      <c r="D37" t="s" s="10">
+        <v>139</v>
+      </c>
+      <c r="E37" t="s" s="10">
+        <v>140</v>
+      </c>
+      <c r="F37" t="s" s="10">
+        <v>128</v>
+      </c>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" ht="20.05" customHeight="1">
+      <c r="A38" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s" s="9">
+        <v>124</v>
+      </c>
+      <c r="C38" t="s" s="10">
+        <v>141</v>
+      </c>
+      <c r="D38" t="s" s="10">
+        <v>142</v>
+      </c>
+      <c r="E38" t="s" s="10">
+        <v>143</v>
+      </c>
+      <c r="F38" t="s" s="10">
+        <v>128</v>
+      </c>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" ht="20.05" customHeight="1">
+      <c r="A39" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="B39" t="s" s="9">
+        <v>124</v>
+      </c>
+      <c r="C39" t="s" s="10">
+        <v>144</v>
+      </c>
+      <c r="D39" t="s" s="10">
+        <v>145</v>
+      </c>
+      <c r="E39" t="s" s="10">
+        <v>146</v>
+      </c>
+      <c r="F39" t="s" s="10">
+        <v>128</v>
+      </c>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" ht="20.05" customHeight="1">
+      <c r="A40" t="s" s="8">
+        <v>147</v>
+      </c>
+      <c r="B40" t="s" s="9">
+        <v>148</v>
+      </c>
+      <c r="C40" t="s" s="10">
+        <v>149</v>
+      </c>
+      <c r="D40" t="s" s="10">
+        <v>150</v>
+      </c>
+      <c r="E40" t="s" s="10">
+        <v>151</v>
+      </c>
+      <c r="F40" t="s" s="10">
+        <v>128</v>
+      </c>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" ht="20.05" customHeight="1">
+      <c r="A41" t="s" s="8">
+        <v>147</v>
+      </c>
+      <c r="B41" t="s" s="9">
+        <v>148</v>
+      </c>
+      <c r="C41" t="s" s="10">
+        <v>152</v>
+      </c>
+      <c r="D41" t="s" s="10">
+        <v>153</v>
+      </c>
+      <c r="E41" t="s" s="10">
+        <v>154</v>
+      </c>
+      <c r="F41" t="s" s="10">
+        <v>89</v>
+      </c>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" ht="20.05" customHeight="1">
+      <c r="A42" t="s" s="8">
+        <v>147</v>
+      </c>
+      <c r="B42" t="s" s="9">
+        <v>148</v>
+      </c>
+      <c r="C42" t="s" s="10">
+        <v>155</v>
+      </c>
+      <c r="D42" t="s" s="10">
+        <v>156</v>
+      </c>
+      <c r="E42" t="s" s="10">
+        <v>157</v>
+      </c>
+      <c r="F42" t="s" s="10">
+        <v>128</v>
+      </c>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" ht="20.05" customHeight="1">
+      <c r="A43" t="s" s="8">
+        <v>147</v>
+      </c>
+      <c r="B43" t="s" s="9">
+        <v>158</v>
+      </c>
+      <c r="C43" t="s" s="10">
+        <v>159</v>
+      </c>
+      <c r="D43" t="s" s="10">
+        <v>160</v>
+      </c>
+      <c r="E43" t="s" s="10">
+        <v>161</v>
+      </c>
+      <c r="F43" t="s" s="10">
         <v>58</v>
       </c>
-      <c r="D16" t="s" s="9">
-        <v>59</v>
-      </c>
-      <c r="E16" t="s" s="9">
-        <v>60</v>
-      </c>
-      <c r="F16" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s" s="9">
-        <v>61</v>
-      </c>
-      <c r="D17" t="s" s="9">
-        <v>62</v>
-      </c>
-      <c r="E17" t="s" s="9">
-        <v>63</v>
-      </c>
-      <c r="F17" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s" s="9">
-        <v>64</v>
-      </c>
-      <c r="D18" t="s" s="9">
-        <v>65</v>
-      </c>
-      <c r="E18" t="s" s="9">
-        <v>66</v>
-      </c>
-      <c r="F18" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="B19" t="s" s="8">
-        <v>68</v>
-      </c>
-      <c r="C19" t="s" s="9">
-        <v>69</v>
-      </c>
-      <c r="D19" t="s" s="9">
-        <v>70</v>
-      </c>
-      <c r="E19" t="s" s="9">
-        <v>71</v>
-      </c>
-      <c r="F19" t="s" s="9">
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" ht="20.05" customHeight="1">
+      <c r="A44" t="s" s="8">
+        <v>147</v>
+      </c>
+      <c r="B44" t="s" s="9">
+        <v>158</v>
+      </c>
+      <c r="C44" t="s" s="10">
+        <v>162</v>
+      </c>
+      <c r="D44" t="s" s="10">
+        <v>163</v>
+      </c>
+      <c r="E44" t="s" s="10">
+        <v>164</v>
+      </c>
+      <c r="F44" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" ht="20.05" customHeight="1">
+      <c r="A45" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B45" t="s" s="9">
+        <v>166</v>
+      </c>
+      <c r="C45" t="s" s="10">
+        <v>167</v>
+      </c>
+      <c r="D45" t="s" s="10">
+        <v>168</v>
+      </c>
+      <c r="E45" t="s" s="10">
+        <v>169</v>
+      </c>
+      <c r="F45" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" ht="20.05" customHeight="1">
+      <c r="A46" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B46" t="s" s="9">
+        <v>166</v>
+      </c>
+      <c r="C46" t="s" s="10">
+        <v>170</v>
+      </c>
+      <c r="D46" t="s" s="10">
+        <v>171</v>
+      </c>
+      <c r="E46" t="s" s="10">
+        <v>172</v>
+      </c>
+      <c r="F46" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" ht="20.05" customHeight="1">
+      <c r="A47" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B47" t="s" s="9">
+        <v>166</v>
+      </c>
+      <c r="C47" t="s" s="10">
+        <v>173</v>
+      </c>
+      <c r="D47" t="s" s="10">
+        <v>174</v>
+      </c>
+      <c r="E47" t="s" s="10">
+        <v>175</v>
+      </c>
+      <c r="F47" t="s" s="10">
+        <v>117</v>
+      </c>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" ht="20.05" customHeight="1">
+      <c r="A48" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B48" t="s" s="9">
+        <v>166</v>
+      </c>
+      <c r="C48" t="s" s="10">
+        <v>176</v>
+      </c>
+      <c r="D48" t="s" s="10">
+        <v>177</v>
+      </c>
+      <c r="E48" t="s" s="10">
+        <v>178</v>
+      </c>
+      <c r="F48" t="s" s="10">
+        <v>117</v>
+      </c>
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" ht="20.05" customHeight="1">
+      <c r="A49" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B49" t="s" s="9">
+        <v>166</v>
+      </c>
+      <c r="C49" t="s" s="10">
+        <v>179</v>
+      </c>
+      <c r="D49" t="s" s="10">
+        <v>180</v>
+      </c>
+      <c r="E49" t="s" s="10">
+        <v>181</v>
+      </c>
+      <c r="F49" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" ht="20.05" customHeight="1">
+      <c r="A50" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B50" t="s" s="9">
+        <v>166</v>
+      </c>
+      <c r="C50" t="s" s="10">
+        <v>182</v>
+      </c>
+      <c r="D50" t="s" s="10">
+        <v>183</v>
+      </c>
+      <c r="E50" t="s" s="10">
+        <v>184</v>
+      </c>
+      <c r="F50" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" ht="20.05" customHeight="1">
+      <c r="A51" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B51" t="s" s="9">
+        <v>166</v>
+      </c>
+      <c r="C51" t="s" s="10">
+        <v>185</v>
+      </c>
+      <c r="D51" t="s" s="10">
+        <v>186</v>
+      </c>
+      <c r="E51" t="s" s="10">
+        <v>187</v>
+      </c>
+      <c r="F51" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" ht="20.05" customHeight="1">
+      <c r="A52" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B52" t="s" s="9">
+        <v>188</v>
+      </c>
+      <c r="C52" t="s" s="10">
+        <v>189</v>
+      </c>
+      <c r="D52" t="s" s="10">
+        <v>190</v>
+      </c>
+      <c r="E52" t="s" s="10">
+        <v>191</v>
+      </c>
+      <c r="F52" t="s" s="10">
+        <v>117</v>
+      </c>
+      <c r="G52" s="10"/>
+    </row>
+    <row r="53" ht="20.05" customHeight="1">
+      <c r="A53" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B53" t="s" s="9">
+        <v>188</v>
+      </c>
+      <c r="C53" t="s" s="10">
+        <v>192</v>
+      </c>
+      <c r="D53" t="s" s="10">
+        <v>193</v>
+      </c>
+      <c r="E53" t="s" s="10">
+        <v>194</v>
+      </c>
+      <c r="F53" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" ht="20.05" customHeight="1">
+      <c r="A54" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B54" t="s" s="9">
+        <v>195</v>
+      </c>
+      <c r="C54" t="s" s="10">
+        <v>196</v>
+      </c>
+      <c r="D54" t="s" s="10">
+        <v>197</v>
+      </c>
+      <c r="E54" t="s" s="10">
+        <v>198</v>
+      </c>
+      <c r="F54" t="s" s="11">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="B20" t="s" s="8">
-        <v>68</v>
-      </c>
-      <c r="C20" t="s" s="9">
-        <v>72</v>
-      </c>
-      <c r="D20" t="s" s="9">
-        <v>73</v>
-      </c>
-      <c r="E20" t="s" s="9">
-        <v>74</v>
-      </c>
-      <c r="F20" t="s" s="9">
+      <c r="G54" s="10"/>
+    </row>
+    <row r="55" ht="20.05" customHeight="1">
+      <c r="A55" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B55" t="s" s="9">
+        <v>195</v>
+      </c>
+      <c r="C55" t="s" s="10">
+        <v>199</v>
+      </c>
+      <c r="D55" t="s" s="10">
+        <v>200</v>
+      </c>
+      <c r="E55" t="s" s="10">
+        <v>201</v>
+      </c>
+      <c r="F55" t="s" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="B21" t="s" s="8">
-        <v>68</v>
-      </c>
-      <c r="C21" t="s" s="9">
-        <v>75</v>
-      </c>
-      <c r="D21" t="s" s="9">
-        <v>76</v>
-      </c>
-      <c r="E21" t="s" s="9">
-        <v>77</v>
-      </c>
-      <c r="F21" t="s" s="9">
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" ht="20.05" customHeight="1">
+      <c r="A56" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B56" t="s" s="9">
+        <v>195</v>
+      </c>
+      <c r="C56" t="s" s="10">
+        <v>202</v>
+      </c>
+      <c r="D56" t="s" s="10">
+        <v>203</v>
+      </c>
+      <c r="E56" t="s" s="10">
+        <v>204</v>
+      </c>
+      <c r="F56" t="s" s="10">
+        <v>117</v>
+      </c>
+      <c r="G56" s="10"/>
+    </row>
+    <row r="57" ht="20.05" customHeight="1">
+      <c r="A57" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B57" t="s" s="9">
+        <v>195</v>
+      </c>
+      <c r="C57" t="s" s="10">
+        <v>205</v>
+      </c>
+      <c r="D57" t="s" s="10">
+        <v>206</v>
+      </c>
+      <c r="E57" t="s" s="10">
+        <v>207</v>
+      </c>
+      <c r="F57" t="s" s="10">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="B22" t="s" s="8">
-        <v>68</v>
-      </c>
-      <c r="C22" t="s" s="9">
-        <v>78</v>
-      </c>
-      <c r="D22" t="s" s="9">
-        <v>79</v>
-      </c>
-      <c r="E22" t="s" s="9">
-        <v>80</v>
-      </c>
-      <c r="F22" t="s" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="B23" t="s" s="8">
-        <v>81</v>
-      </c>
-      <c r="C23" t="s" s="9">
-        <v>82</v>
-      </c>
-      <c r="D23" t="s" s="9">
-        <v>83</v>
-      </c>
-      <c r="E23" t="s" s="9">
-        <v>84</v>
-      </c>
-      <c r="F23" t="s" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="B24" t="s" s="8">
-        <v>81</v>
-      </c>
-      <c r="C24" t="s" s="9">
-        <v>85</v>
-      </c>
-      <c r="D24" t="s" s="9">
-        <v>86</v>
-      </c>
-      <c r="E24" t="s" s="9">
-        <v>87</v>
-      </c>
-      <c r="F24" t="s" s="9">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="B25" t="s" s="8">
-        <v>81</v>
-      </c>
-      <c r="C25" t="s" s="9">
-        <v>89</v>
-      </c>
-      <c r="D25" t="s" s="9">
-        <v>90</v>
-      </c>
-      <c r="E25" t="s" s="9">
-        <v>91</v>
-      </c>
-      <c r="F25" t="s" s="9">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="7">
-        <v>92</v>
-      </c>
-      <c r="B26" t="s" s="8">
-        <v>93</v>
-      </c>
-      <c r="C26" t="s" s="9">
-        <v>94</v>
-      </c>
-      <c r="D26" t="s" s="9">
-        <v>95</v>
-      </c>
-      <c r="E26" t="s" s="9">
-        <v>96</v>
-      </c>
-      <c r="F26" t="s" s="9">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" t="s" s="7">
-        <v>92</v>
-      </c>
-      <c r="B27" t="s" s="8">
-        <v>93</v>
-      </c>
-      <c r="C27" t="s" s="9">
-        <v>97</v>
-      </c>
-      <c r="D27" t="s" s="9">
-        <v>98</v>
-      </c>
-      <c r="E27" t="s" s="9">
-        <v>99</v>
-      </c>
-      <c r="F27" t="s" s="9">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" t="s" s="7">
-        <v>92</v>
-      </c>
-      <c r="B28" t="s" s="8">
-        <v>93</v>
-      </c>
-      <c r="C28" t="s" s="9">
-        <v>100</v>
-      </c>
-      <c r="D28" t="s" s="9">
-        <v>101</v>
-      </c>
-      <c r="E28" t="s" s="9">
-        <v>102</v>
-      </c>
-      <c r="F28" t="s" s="9">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" t="s" s="7">
-        <v>92</v>
-      </c>
-      <c r="B29" t="s" s="8">
-        <v>103</v>
-      </c>
-      <c r="C29" t="s" s="9">
-        <v>104</v>
-      </c>
-      <c r="D29" t="s" s="9">
-        <v>105</v>
-      </c>
-      <c r="E29" t="s" s="9">
-        <v>106</v>
-      </c>
-      <c r="F29" t="s" s="9">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B30" t="s" s="8">
-        <v>108</v>
-      </c>
-      <c r="C30" t="s" s="9">
-        <v>109</v>
-      </c>
-      <c r="D30" t="s" s="9">
-        <v>110</v>
-      </c>
-      <c r="E30" t="s" s="9">
-        <v>111</v>
-      </c>
-      <c r="F30" t="s" s="9">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B31" t="s" s="8">
-        <v>108</v>
-      </c>
-      <c r="C31" t="s" s="9">
+      <c r="G57" s="10"/>
+    </row>
+    <row r="58" ht="20.05" customHeight="1">
+      <c r="A58" t="s" s="8">
+        <v>165</v>
+      </c>
+      <c r="B58" t="s" s="9">
+        <v>208</v>
+      </c>
+      <c r="C58" t="s" s="10">
+        <v>209</v>
+      </c>
+      <c r="D58" t="s" s="10">
+        <v>210</v>
+      </c>
+      <c r="E58" t="s" s="10">
+        <v>211</v>
+      </c>
+      <c r="F58" t="s" s="10">
         <v>113</v>
       </c>
-      <c r="D31" t="s" s="9">
-        <v>114</v>
-      </c>
-      <c r="E31" t="s" s="9">
-        <v>115</v>
-      </c>
-      <c r="F31" t="s" s="9">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B32" t="s" s="8">
-        <v>108</v>
-      </c>
-      <c r="C32" t="s" s="9">
-        <v>117</v>
-      </c>
-      <c r="D32" t="s" s="9">
-        <v>118</v>
-      </c>
-      <c r="E32" t="s" s="9">
-        <v>119</v>
-      </c>
-      <c r="F32" t="s" s="9">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B33" t="s" s="8">
-        <v>108</v>
-      </c>
-      <c r="C33" t="s" s="9">
-        <v>120</v>
-      </c>
-      <c r="D33" t="s" s="9">
-        <v>121</v>
-      </c>
-      <c r="E33" t="s" s="9">
-        <v>122</v>
-      </c>
-      <c r="F33" t="s" s="9">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B34" t="s" s="8">
-        <v>123</v>
-      </c>
-      <c r="C34" t="s" s="9">
-        <v>124</v>
-      </c>
-      <c r="D34" t="s" s="9">
-        <v>125</v>
-      </c>
-      <c r="E34" t="s" s="9">
-        <v>126</v>
-      </c>
-      <c r="F34" t="s" s="9">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" ht="20.05" customHeight="1">
-      <c r="A35" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B35" t="s" s="8">
-        <v>123</v>
-      </c>
-      <c r="C35" t="s" s="9">
-        <v>128</v>
-      </c>
-      <c r="D35" t="s" s="9">
-        <v>129</v>
-      </c>
-      <c r="E35" t="s" s="9">
-        <v>130</v>
-      </c>
-      <c r="F35" t="s" s="9">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B36" t="s" s="8">
-        <v>123</v>
-      </c>
-      <c r="C36" t="s" s="9">
-        <v>131</v>
-      </c>
-      <c r="D36" t="s" s="9">
-        <v>132</v>
-      </c>
-      <c r="E36" t="s" s="9">
-        <v>133</v>
-      </c>
-      <c r="F36" t="s" s="9">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="37" ht="20.05" customHeight="1">
-      <c r="A37" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B37" t="s" s="8">
-        <v>123</v>
-      </c>
-      <c r="C37" t="s" s="9">
-        <v>134</v>
-      </c>
-      <c r="D37" t="s" s="9">
-        <v>135</v>
-      </c>
-      <c r="E37" t="s" s="9">
-        <v>136</v>
-      </c>
-      <c r="F37" t="s" s="9">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" ht="20.05" customHeight="1">
-      <c r="A38" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B38" t="s" s="8">
-        <v>123</v>
-      </c>
-      <c r="C38" t="s" s="9">
-        <v>137</v>
-      </c>
-      <c r="D38" t="s" s="9">
-        <v>138</v>
-      </c>
-      <c r="E38" t="s" s="9">
-        <v>139</v>
-      </c>
-      <c r="F38" t="s" s="9">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B39" t="s" s="8">
-        <v>123</v>
-      </c>
-      <c r="C39" t="s" s="9">
-        <v>140</v>
-      </c>
-      <c r="D39" t="s" s="9">
-        <v>141</v>
-      </c>
-      <c r="E39" t="s" s="9">
-        <v>142</v>
-      </c>
-      <c r="F39" t="s" s="9">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B40" t="s" s="8">
-        <v>123</v>
-      </c>
-      <c r="C40" t="s" s="9">
-        <v>143</v>
-      </c>
-      <c r="D40" t="s" s="9">
-        <v>144</v>
-      </c>
-      <c r="E40" t="s" s="9">
-        <v>145</v>
-      </c>
-      <c r="F40" t="s" s="9">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" t="s" s="7">
-        <v>146</v>
-      </c>
-      <c r="B41" t="s" s="8">
-        <v>147</v>
-      </c>
-      <c r="C41" t="s" s="9">
-        <v>148</v>
-      </c>
-      <c r="D41" t="s" s="9">
-        <v>149</v>
-      </c>
-      <c r="E41" t="s" s="9">
-        <v>150</v>
-      </c>
-      <c r="F41" t="s" s="9">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" t="s" s="7">
-        <v>146</v>
-      </c>
-      <c r="B42" t="s" s="8">
-        <v>147</v>
-      </c>
-      <c r="C42" t="s" s="9">
-        <v>151</v>
-      </c>
-      <c r="D42" t="s" s="9">
-        <v>152</v>
-      </c>
-      <c r="E42" t="s" s="9">
-        <v>153</v>
-      </c>
-      <c r="F42" t="s" s="9">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" ht="20.05" customHeight="1">
-      <c r="A43" t="s" s="7">
-        <v>146</v>
-      </c>
-      <c r="B43" t="s" s="8">
-        <v>147</v>
-      </c>
-      <c r="C43" t="s" s="9">
-        <v>154</v>
-      </c>
-      <c r="D43" t="s" s="9">
-        <v>155</v>
-      </c>
-      <c r="E43" t="s" s="9">
-        <v>156</v>
-      </c>
-      <c r="F43" t="s" s="9">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" ht="20.05" customHeight="1">
-      <c r="A44" t="s" s="7">
-        <v>146</v>
-      </c>
-      <c r="B44" t="s" s="8">
-        <v>157</v>
-      </c>
-      <c r="C44" t="s" s="9">
-        <v>158</v>
-      </c>
-      <c r="D44" t="s" s="9">
-        <v>159</v>
-      </c>
-      <c r="E44" t="s" s="9">
-        <v>160</v>
-      </c>
-      <c r="F44" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" t="s" s="7">
-        <v>146</v>
-      </c>
-      <c r="B45" t="s" s="8">
-        <v>157</v>
-      </c>
-      <c r="C45" t="s" s="9">
-        <v>161</v>
-      </c>
-      <c r="D45" t="s" s="9">
-        <v>162</v>
-      </c>
-      <c r="E45" t="s" s="9">
-        <v>163</v>
-      </c>
-      <c r="F45" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B46" t="s" s="8">
-        <v>165</v>
-      </c>
-      <c r="C46" t="s" s="9">
-        <v>166</v>
-      </c>
-      <c r="D46" t="s" s="9">
-        <v>167</v>
-      </c>
-      <c r="E46" t="s" s="9">
-        <v>168</v>
-      </c>
-      <c r="F46" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B47" t="s" s="8">
-        <v>165</v>
-      </c>
-      <c r="C47" t="s" s="9">
-        <v>169</v>
-      </c>
-      <c r="D47" t="s" s="9">
-        <v>170</v>
-      </c>
-      <c r="E47" t="s" s="9">
-        <v>171</v>
-      </c>
-      <c r="F47" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B48" t="s" s="8">
-        <v>165</v>
-      </c>
-      <c r="C48" t="s" s="9">
-        <v>172</v>
-      </c>
-      <c r="D48" t="s" s="9">
-        <v>173</v>
-      </c>
-      <c r="E48" t="s" s="9">
-        <v>174</v>
-      </c>
-      <c r="F48" t="s" s="9">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B49" t="s" s="8">
-        <v>165</v>
-      </c>
-      <c r="C49" t="s" s="9">
-        <v>175</v>
-      </c>
-      <c r="D49" t="s" s="9">
-        <v>176</v>
-      </c>
-      <c r="E49" t="s" s="9">
-        <v>177</v>
-      </c>
-      <c r="F49" t="s" s="9">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B50" t="s" s="8">
-        <v>165</v>
-      </c>
-      <c r="C50" t="s" s="9">
-        <v>178</v>
-      </c>
-      <c r="D50" t="s" s="9">
-        <v>179</v>
-      </c>
-      <c r="E50" t="s" s="9">
-        <v>180</v>
-      </c>
-      <c r="F50" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B51" t="s" s="8">
-        <v>165</v>
-      </c>
-      <c r="C51" t="s" s="9">
-        <v>181</v>
-      </c>
-      <c r="D51" t="s" s="9">
-        <v>182</v>
-      </c>
-      <c r="E51" t="s" s="9">
-        <v>183</v>
-      </c>
-      <c r="F51" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="52" ht="20.05" customHeight="1">
-      <c r="A52" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B52" t="s" s="8">
-        <v>165</v>
-      </c>
-      <c r="C52" t="s" s="9">
-        <v>184</v>
-      </c>
-      <c r="D52" t="s" s="9">
-        <v>185</v>
-      </c>
-      <c r="E52" t="s" s="9">
-        <v>186</v>
-      </c>
-      <c r="F52" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" ht="20.05" customHeight="1">
-      <c r="A53" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B53" t="s" s="8">
-        <v>187</v>
-      </c>
-      <c r="C53" t="s" s="9">
-        <v>188</v>
-      </c>
-      <c r="D53" t="s" s="9">
-        <v>189</v>
-      </c>
-      <c r="E53" t="s" s="9">
-        <v>190</v>
-      </c>
-      <c r="F53" t="s" s="9">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" ht="20.05" customHeight="1">
-      <c r="A54" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B54" t="s" s="8">
-        <v>187</v>
-      </c>
-      <c r="C54" t="s" s="9">
-        <v>191</v>
-      </c>
-      <c r="D54" t="s" s="9">
-        <v>192</v>
-      </c>
-      <c r="E54" t="s" s="9">
-        <v>193</v>
-      </c>
-      <c r="F54" t="s" s="9">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" ht="20.05" customHeight="1">
-      <c r="A55" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B55" t="s" s="8">
-        <v>194</v>
-      </c>
-      <c r="C55" t="s" s="9">
-        <v>195</v>
-      </c>
-      <c r="D55" t="s" s="9">
-        <v>196</v>
-      </c>
-      <c r="E55" t="s" s="9">
-        <v>197</v>
-      </c>
-      <c r="F55" t="s" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" ht="20.05" customHeight="1">
-      <c r="A56" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B56" t="s" s="8">
-        <v>194</v>
-      </c>
-      <c r="C56" t="s" s="9">
-        <v>198</v>
-      </c>
-      <c r="D56" t="s" s="9">
-        <v>199</v>
-      </c>
-      <c r="E56" t="s" s="9">
-        <v>200</v>
-      </c>
-      <c r="F56" t="s" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" ht="20.05" customHeight="1">
-      <c r="A57" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B57" t="s" s="8">
-        <v>194</v>
-      </c>
-      <c r="C57" t="s" s="9">
-        <v>201</v>
-      </c>
-      <c r="D57" t="s" s="9">
-        <v>202</v>
-      </c>
-      <c r="E57" t="s" s="9">
-        <v>203</v>
-      </c>
-      <c r="F57" t="s" s="9">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" ht="20.05" customHeight="1">
-      <c r="A58" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B58" t="s" s="8">
-        <v>194</v>
-      </c>
-      <c r="C58" t="s" s="9">
-        <v>204</v>
-      </c>
-      <c r="D58" t="s" s="9">
-        <v>205</v>
-      </c>
-      <c r="E58" t="s" s="9">
-        <v>206</v>
-      </c>
-      <c r="F58" t="s" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" ht="20.05" customHeight="1">
-      <c r="A59" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="B59" t="s" s="8">
-        <v>207</v>
-      </c>
-      <c r="C59" t="s" s="9">
-        <v>208</v>
-      </c>
-      <c r="D59" t="s" s="9">
-        <v>209</v>
-      </c>
-      <c r="E59" t="s" s="9">
-        <v>210</v>
-      </c>
-      <c r="F59" t="s" s="9">
-        <v>112</v>
-      </c>
+      <c r="G58" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" location="" tooltip="" display="Gartner - AI Roadmap Toolkit (public) | https://www.gartner.com/en/chief-information-officer/research/ai-maturity-model-toolkit || &#10;Gartner - AI Strategy Reference Guide (internal) | https://www.gartner.com/document-reader/document/5938007?ref=pubsite || &#10;Gartner - AI Strategy for Business (public) | https://www.gartner.com/en/articles/ai-strategy-for-business || &#10;Gartner - The Pillars of a Successful Artificial Intelligence Strategy (internal) | https://www.gartner.com/document-reader/document/5373763? || &#10;Gartner - Reference Guide for AI Strategy (internal) | https://www.gartner.com/document-reader/document/6676234?ref=pubsite || &#10;ISO/IEC 42001:2023 - Information technology — Artificial intelligence — Management syste (public) | https://www.iso.org/standard/42001 || &#10;NIST - AI Risk Management Framework (public) | https://www.nist.gov/itl/ai-risk-management-framework"/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>